<commit_message>
Added COPD, excessive heat, and built housing years, updated preprocessing script - need to check character to numeric.
</commit_message>
<xml_diff>
--- a/data/processed/Data_Dictionary.xlsx
+++ b/data/processed/Data_Dictionary.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/davidmccoy/COVIDxrisk/data/processed/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E4BAF790-561E-EA45-A361-FA232BC85057}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DB0F8F63-E980-5B4F-959B-D369C8BC270D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="31480" yWindow="1040" windowWidth="45420" windowHeight="23040" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="30820" yWindow="620" windowWidth="45420" windowHeight="23040" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Table 1" sheetId="1" r:id="rId1"/>
@@ -20,12 +20,12 @@
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">'Table 1'!$A$1:$K$180</definedName>
   </definedNames>
-  <calcPr calcId="181029" concurrentCalc="0"/>
+  <calcPr calcId="181029"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3101" uniqueCount="930">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3131" uniqueCount="942">
   <si>
     <t>Col Num</t>
   </si>
@@ -3577,6 +3577,42 @@
   </si>
   <si>
     <t>Label</t>
+  </si>
+  <si>
+    <t>ex_heat_count_mean</t>
+  </si>
+  <si>
+    <t>Mean Excessive Heat Count</t>
+  </si>
+  <si>
+    <t>UV_ Wh/m²</t>
+  </si>
+  <si>
+    <t>UV Wh/m²</t>
+  </si>
+  <si>
+    <t>COPD_mean</t>
+  </si>
+  <si>
+    <t>Mean Percentage COPD</t>
+  </si>
+  <si>
+    <t>mean_before1950</t>
+  </si>
+  <si>
+    <t>mean_between1950_75</t>
+  </si>
+  <si>
+    <t>mean_before1980</t>
+  </si>
+  <si>
+    <t>Mean Percentage Housing Built Before 1950</t>
+  </si>
+  <si>
+    <t>Mean Percentage Housing Built Between 1950-75</t>
+  </si>
+  <si>
+    <t>Mean Percentage Housing Built Before 1980</t>
   </si>
 </sst>
 </file>
@@ -4289,10 +4325,10 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <sheetPr filterMode="1"/>
-  <dimension ref="A1:K419"/>
+  <dimension ref="A1:K425"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="112" workbookViewId="0">
-      <selection activeCell="F2" sqref="F2"/>
+    <sheetView tabSelected="1" topLeftCell="A92" zoomScale="112" workbookViewId="0">
+      <selection activeCell="E101" sqref="E101"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="20.19921875" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
@@ -14206,6 +14242,108 @@
         <v>886</v>
       </c>
       <c r="J419" s="6" t="s">
+        <v>254</v>
+      </c>
+    </row>
+    <row r="420" spans="2:10" ht="14" x14ac:dyDescent="0.15">
+      <c r="B420" s="6" t="s">
+        <v>930</v>
+      </c>
+      <c r="C420" s="6" t="s">
+        <v>931</v>
+      </c>
+      <c r="F420" s="6" t="s">
+        <v>928</v>
+      </c>
+      <c r="G420" s="6" t="s">
+        <v>928</v>
+      </c>
+      <c r="J420" s="6" t="s">
+        <v>254</v>
+      </c>
+    </row>
+    <row r="421" spans="2:10" ht="14" x14ac:dyDescent="0.15">
+      <c r="B421" s="6" t="s">
+        <v>932</v>
+      </c>
+      <c r="C421" s="6" t="s">
+        <v>933</v>
+      </c>
+      <c r="F421" s="6" t="s">
+        <v>928</v>
+      </c>
+      <c r="G421" s="6" t="s">
+        <v>928</v>
+      </c>
+      <c r="J421" s="6" t="s">
+        <v>254</v>
+      </c>
+    </row>
+    <row r="422" spans="2:10" ht="14" x14ac:dyDescent="0.15">
+      <c r="B422" s="6" t="s">
+        <v>934</v>
+      </c>
+      <c r="C422" s="6" t="s">
+        <v>935</v>
+      </c>
+      <c r="F422" s="2" t="s">
+        <v>48</v>
+      </c>
+      <c r="G422" s="2" t="s">
+        <v>48</v>
+      </c>
+      <c r="J422" s="6" t="s">
+        <v>254</v>
+      </c>
+    </row>
+    <row r="423" spans="2:10" ht="14" x14ac:dyDescent="0.15">
+      <c r="B423" s="6" t="s">
+        <v>936</v>
+      </c>
+      <c r="C423" s="6" t="s">
+        <v>939</v>
+      </c>
+      <c r="F423" s="3" t="s">
+        <v>923</v>
+      </c>
+      <c r="G423" s="3" t="s">
+        <v>923</v>
+      </c>
+      <c r="J423" s="6" t="s">
+        <v>254</v>
+      </c>
+    </row>
+    <row r="424" spans="2:10" ht="14" x14ac:dyDescent="0.15">
+      <c r="B424" s="6" t="s">
+        <v>937</v>
+      </c>
+      <c r="C424" s="6" t="s">
+        <v>940</v>
+      </c>
+      <c r="F424" s="3" t="s">
+        <v>923</v>
+      </c>
+      <c r="G424" s="3" t="s">
+        <v>923</v>
+      </c>
+      <c r="J424" s="6" t="s">
+        <v>254</v>
+      </c>
+    </row>
+    <row r="425" spans="2:10" ht="14" x14ac:dyDescent="0.15">
+      <c r="B425" s="6" t="s">
+        <v>938</v>
+      </c>
+      <c r="C425" s="6" t="s">
+        <v>941</v>
+      </c>
+      <c r="F425" s="3" t="s">
+        <v>923</v>
+      </c>
+      <c r="G425" s="3" t="s">
+        <v>923</v>
+      </c>
+      <c r="J425" s="6" t="s">
         <v>254</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Fixing scripts for server
</commit_message>
<xml_diff>
--- a/data/processed/Data_Dictionary.xlsx
+++ b/data/processed/Data_Dictionary.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/davidmccoy/COVIDxrisk/data/processed/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DB0F8F63-E980-5B4F-959B-D369C8BC270D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{83F8A790-B5FE-7447-A8C1-70D811F32E66}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="30820" yWindow="620" windowWidth="45420" windowHeight="23040" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="16060" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Table 1" sheetId="1" r:id="rId1"/>
@@ -3585,9 +3585,6 @@
     <t>Mean Excessive Heat Count</t>
   </si>
   <si>
-    <t>UV_ Wh/m²</t>
-  </si>
-  <si>
     <t>UV Wh/m²</t>
   </si>
   <si>
@@ -3613,6 +3610,9 @@
   </si>
   <si>
     <t>Mean Percentage Housing Built Before 1980</t>
+  </si>
+  <si>
+    <t>UV_metric</t>
   </si>
 </sst>
 </file>
@@ -4327,8 +4327,8 @@
   <sheetPr filterMode="1"/>
   <dimension ref="A1:K425"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A92" zoomScale="112" workbookViewId="0">
-      <selection activeCell="E101" sqref="E101"/>
+    <sheetView tabSelected="1" topLeftCell="A412" zoomScale="112" workbookViewId="0">
+      <selection activeCell="B420" sqref="B420"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="20.19921875" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
@@ -14264,10 +14264,10 @@
     </row>
     <row r="421" spans="2:10" ht="14" x14ac:dyDescent="0.15">
       <c r="B421" s="6" t="s">
+        <v>941</v>
+      </c>
+      <c r="C421" s="6" t="s">
         <v>932</v>
-      </c>
-      <c r="C421" s="6" t="s">
-        <v>933</v>
       </c>
       <c r="F421" s="6" t="s">
         <v>928</v>
@@ -14281,10 +14281,10 @@
     </row>
     <row r="422" spans="2:10" ht="14" x14ac:dyDescent="0.15">
       <c r="B422" s="6" t="s">
+        <v>933</v>
+      </c>
+      <c r="C422" s="6" t="s">
         <v>934</v>
-      </c>
-      <c r="C422" s="6" t="s">
-        <v>935</v>
       </c>
       <c r="F422" s="2" t="s">
         <v>48</v>
@@ -14298,10 +14298,10 @@
     </row>
     <row r="423" spans="2:10" ht="14" x14ac:dyDescent="0.15">
       <c r="B423" s="6" t="s">
-        <v>936</v>
+        <v>935</v>
       </c>
       <c r="C423" s="6" t="s">
-        <v>939</v>
+        <v>938</v>
       </c>
       <c r="F423" s="3" t="s">
         <v>923</v>
@@ -14315,10 +14315,10 @@
     </row>
     <row r="424" spans="2:10" ht="14" x14ac:dyDescent="0.15">
       <c r="B424" s="6" t="s">
-        <v>937</v>
+        <v>936</v>
       </c>
       <c r="C424" s="6" t="s">
-        <v>940</v>
+        <v>939</v>
       </c>
       <c r="F424" s="3" t="s">
         <v>923</v>
@@ -14332,10 +14332,10 @@
     </row>
     <row r="425" spans="2:10" ht="14" x14ac:dyDescent="0.15">
       <c r="B425" s="6" t="s">
-        <v>938</v>
+        <v>937</v>
       </c>
       <c r="C425" s="6" t="s">
-        <v>941</v>
+        <v>940</v>
       </c>
       <c r="F425" s="3" t="s">
         <v>923</v>

</xml_diff>

<commit_message>
Updated modeling scripts to include sub-categories plot.
</commit_message>
<xml_diff>
--- a/data/processed/Data_Dictionary.xlsx
+++ b/data/processed/Data_Dictionary.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/davidmccoy/COVIDxrisk/data/processed/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{83F8A790-B5FE-7447-A8C1-70D811F32E66}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2CB85E68-F47A-534E-86F8-B1550109FD46}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="16060" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="31700" yWindow="760" windowWidth="44820" windowHeight="20900" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Table 1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3131" uniqueCount="942">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3131" uniqueCount="945">
   <si>
     <t>Col Num</t>
   </si>
@@ -3567,9 +3567,6 @@
     <t>Racism</t>
   </si>
   <si>
-    <t>Health</t>
-  </si>
-  <si>
     <t>Education/Employment</t>
   </si>
   <si>
@@ -3613,6 +3610,18 @@
   </si>
   <si>
     <t>UV_metric</t>
+  </si>
+  <si>
+    <t>Pesticides</t>
+  </si>
+  <si>
+    <t>Water Toxicants</t>
+  </si>
+  <si>
+    <t>Other Pollutants</t>
+  </si>
+  <si>
+    <t>Air Pollution</t>
   </si>
 </sst>
 </file>
@@ -4327,8 +4336,8 @@
   <sheetPr filterMode="1"/>
   <dimension ref="A1:K425"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A412" zoomScale="112" workbookViewId="0">
-      <selection activeCell="B420" sqref="B420"/>
+    <sheetView tabSelected="1" topLeftCell="A4" zoomScale="112" workbookViewId="0">
+      <selection activeCell="F103" sqref="F103"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="20.19921875" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
@@ -4359,7 +4368,7 @@
         <v>382</v>
       </c>
       <c r="F1" s="10" t="s">
-        <v>929</v>
+        <v>928</v>
       </c>
       <c r="G1" s="11" t="s">
         <v>258</v>
@@ -7330,7 +7339,7 @@
         <v>5</v>
       </c>
       <c r="F95" s="4" t="s">
-        <v>927</v>
+        <v>926</v>
       </c>
       <c r="G95" s="4" t="s">
         <v>357</v>
@@ -7571,7 +7580,7 @@
         <v>17</v>
       </c>
       <c r="F103" s="3" t="s">
-        <v>923</v>
+        <v>944</v>
       </c>
       <c r="G103" s="3" t="s">
         <v>250</v>
@@ -7690,7 +7699,7 @@
         <v>17</v>
       </c>
       <c r="F107" s="3" t="s">
-        <v>923</v>
+        <v>944</v>
       </c>
       <c r="G107" s="3" t="s">
         <v>250</v>
@@ -7722,7 +7731,7 @@
         <v>17</v>
       </c>
       <c r="F108" s="3" t="s">
-        <v>923</v>
+        <v>942</v>
       </c>
       <c r="G108" s="3" t="s">
         <v>250</v>
@@ -7752,7 +7761,7 @@
         <v>17</v>
       </c>
       <c r="F109" s="3" t="s">
-        <v>928</v>
+        <v>927</v>
       </c>
       <c r="G109" s="3" t="s">
         <v>250</v>
@@ -7785,7 +7794,7 @@
         <v>17</v>
       </c>
       <c r="F110" s="3" t="s">
-        <v>928</v>
+        <v>927</v>
       </c>
       <c r="G110" s="3" t="s">
         <v>250</v>
@@ -7818,7 +7827,7 @@
         <v>17</v>
       </c>
       <c r="F111" s="3" t="s">
-        <v>928</v>
+        <v>927</v>
       </c>
       <c r="G111" s="3" t="s">
         <v>250</v>
@@ -7851,7 +7860,7 @@
         <v>5</v>
       </c>
       <c r="F112" s="3" t="s">
-        <v>928</v>
+        <v>927</v>
       </c>
       <c r="G112" s="3" t="s">
         <v>250</v>
@@ -7881,7 +7890,7 @@
         <v>5</v>
       </c>
       <c r="F113" s="3" t="s">
-        <v>928</v>
+        <v>927</v>
       </c>
       <c r="G113" s="3" t="s">
         <v>250</v>
@@ -7911,7 +7920,7 @@
         <v>5</v>
       </c>
       <c r="F114" s="3" t="s">
-        <v>928</v>
+        <v>927</v>
       </c>
       <c r="G114" s="3" t="s">
         <v>250</v>
@@ -7941,7 +7950,7 @@
         <v>5</v>
       </c>
       <c r="F115" s="3" t="s">
-        <v>928</v>
+        <v>927</v>
       </c>
       <c r="G115" s="3" t="s">
         <v>250</v>
@@ -7971,7 +7980,7 @@
         <v>5</v>
       </c>
       <c r="F116" s="3" t="s">
-        <v>928</v>
+        <v>927</v>
       </c>
       <c r="G116" s="3" t="s">
         <v>250</v>
@@ -8003,7 +8012,7 @@
         <v>17</v>
       </c>
       <c r="F117" s="3" t="s">
-        <v>928</v>
+        <v>927</v>
       </c>
       <c r="G117" s="3" t="s">
         <v>250</v>
@@ -8033,7 +8042,7 @@
         <v>17</v>
       </c>
       <c r="F118" s="3" t="s">
-        <v>928</v>
+        <v>927</v>
       </c>
       <c r="G118" s="3" t="s">
         <v>250</v>
@@ -8063,7 +8072,7 @@
         <v>17</v>
       </c>
       <c r="F119" s="3" t="s">
-        <v>928</v>
+        <v>927</v>
       </c>
       <c r="G119" s="3" t="s">
         <v>250</v>
@@ -8093,7 +8102,7 @@
         <v>17</v>
       </c>
       <c r="F120" s="3" t="s">
-        <v>928</v>
+        <v>927</v>
       </c>
       <c r="G120" s="3" t="s">
         <v>250</v>
@@ -8125,7 +8134,7 @@
         <v>17</v>
       </c>
       <c r="F121" s="64" t="s">
-        <v>927</v>
+        <v>926</v>
       </c>
       <c r="G121" s="2" t="s">
         <v>361</v>
@@ -8157,7 +8166,7 @@
         <v>17</v>
       </c>
       <c r="F122" s="64" t="s">
-        <v>927</v>
+        <v>926</v>
       </c>
       <c r="G122" s="2" t="s">
         <v>361</v>
@@ -8189,7 +8198,7 @@
         <v>17</v>
       </c>
       <c r="F123" s="64" t="s">
-        <v>927</v>
+        <v>926</v>
       </c>
       <c r="G123" s="2" t="s">
         <v>357</v>
@@ -8221,7 +8230,7 @@
         <v>17</v>
       </c>
       <c r="F124" s="64" t="s">
-        <v>927</v>
+        <v>926</v>
       </c>
       <c r="G124" s="14" t="s">
         <v>363</v>
@@ -8253,7 +8262,7 @@
         <v>17</v>
       </c>
       <c r="F125" s="64" t="s">
-        <v>927</v>
+        <v>926</v>
       </c>
       <c r="G125" s="14" t="s">
         <v>363</v>
@@ -9717,7 +9726,7 @@
         <v>415</v>
       </c>
       <c r="F177" s="6" t="s">
-        <v>926</v>
+        <v>48</v>
       </c>
       <c r="G177" s="3" t="s">
         <v>249</v>
@@ -9749,7 +9758,7 @@
         <v>415</v>
       </c>
       <c r="F178" s="6" t="s">
-        <v>926</v>
+        <v>48</v>
       </c>
       <c r="G178" s="6" t="s">
         <v>280</v>
@@ -9781,7 +9790,7 @@
         <v>415</v>
       </c>
       <c r="F179" s="6" t="s">
-        <v>926</v>
+        <v>48</v>
       </c>
       <c r="G179" s="6" t="s">
         <v>262</v>
@@ -9813,7 +9822,7 @@
         <v>415</v>
       </c>
       <c r="F180" s="6" t="s">
-        <v>926</v>
+        <v>48</v>
       </c>
       <c r="G180" s="6" t="s">
         <v>262</v>
@@ -9992,7 +10001,7 @@
         <v>802</v>
       </c>
       <c r="F187" s="3" t="s">
-        <v>923</v>
+        <v>941</v>
       </c>
       <c r="G187" s="6" t="s">
         <v>521</v>
@@ -10012,7 +10021,7 @@
         <v>803</v>
       </c>
       <c r="F188" s="3" t="s">
-        <v>923</v>
+        <v>941</v>
       </c>
       <c r="G188" s="6" t="s">
         <v>521</v>
@@ -10032,7 +10041,7 @@
         <v>804</v>
       </c>
       <c r="F189" s="3" t="s">
-        <v>923</v>
+        <v>941</v>
       </c>
       <c r="G189" s="6" t="s">
         <v>521</v>
@@ -10052,7 +10061,7 @@
         <v>805</v>
       </c>
       <c r="F190" s="3" t="s">
-        <v>923</v>
+        <v>941</v>
       </c>
       <c r="G190" s="6" t="s">
         <v>521</v>
@@ -10072,7 +10081,7 @@
         <v>806</v>
       </c>
       <c r="F191" s="3" t="s">
-        <v>923</v>
+        <v>941</v>
       </c>
       <c r="G191" s="6" t="s">
         <v>521</v>
@@ -10092,7 +10101,7 @@
         <v>807</v>
       </c>
       <c r="F192" s="3" t="s">
-        <v>923</v>
+        <v>941</v>
       </c>
       <c r="G192" s="6" t="s">
         <v>521</v>
@@ -10112,7 +10121,7 @@
         <v>432</v>
       </c>
       <c r="F193" s="3" t="s">
-        <v>923</v>
+        <v>941</v>
       </c>
       <c r="G193" s="6" t="s">
         <v>437</v>
@@ -10132,7 +10141,7 @@
         <v>433</v>
       </c>
       <c r="F194" s="3" t="s">
-        <v>923</v>
+        <v>941</v>
       </c>
       <c r="G194" s="6" t="s">
         <v>437</v>
@@ -10152,7 +10161,7 @@
         <v>434</v>
       </c>
       <c r="F195" s="3" t="s">
-        <v>923</v>
+        <v>941</v>
       </c>
       <c r="G195" s="6" t="s">
         <v>437</v>
@@ -10172,7 +10181,7 @@
         <v>435</v>
       </c>
       <c r="F196" s="3" t="s">
-        <v>923</v>
+        <v>941</v>
       </c>
       <c r="G196" s="6" t="s">
         <v>437</v>
@@ -10192,7 +10201,7 @@
         <v>436</v>
       </c>
       <c r="F197" s="3" t="s">
-        <v>923</v>
+        <v>941</v>
       </c>
       <c r="G197" s="6" t="s">
         <v>437</v>
@@ -10212,7 +10221,7 @@
         <v>443</v>
       </c>
       <c r="F198" s="3" t="s">
-        <v>923</v>
+        <v>941</v>
       </c>
       <c r="G198" s="6" t="s">
         <v>522</v>
@@ -10232,7 +10241,7 @@
         <v>448</v>
       </c>
       <c r="F199" s="3" t="s">
-        <v>923</v>
+        <v>941</v>
       </c>
       <c r="G199" s="6" t="s">
         <v>522</v>
@@ -10252,7 +10261,7 @@
         <v>453</v>
       </c>
       <c r="F200" s="3" t="s">
-        <v>923</v>
+        <v>941</v>
       </c>
       <c r="G200" s="6" t="s">
         <v>522</v>
@@ -10272,7 +10281,7 @@
         <v>458</v>
       </c>
       <c r="F201" s="3" t="s">
-        <v>923</v>
+        <v>941</v>
       </c>
       <c r="G201" s="6" t="s">
         <v>522</v>
@@ -10292,7 +10301,7 @@
         <v>463</v>
       </c>
       <c r="F202" s="3" t="s">
-        <v>923</v>
+        <v>941</v>
       </c>
       <c r="G202" s="6" t="s">
         <v>522</v>
@@ -10312,7 +10321,7 @@
         <v>468</v>
       </c>
       <c r="F203" s="3" t="s">
-        <v>923</v>
+        <v>941</v>
       </c>
       <c r="G203" s="6" t="s">
         <v>522</v>
@@ -10332,7 +10341,7 @@
         <v>473</v>
       </c>
       <c r="F204" s="3" t="s">
-        <v>923</v>
+        <v>941</v>
       </c>
       <c r="G204" s="6" t="s">
         <v>522</v>
@@ -10352,7 +10361,7 @@
         <v>478</v>
       </c>
       <c r="F205" s="3" t="s">
-        <v>923</v>
+        <v>941</v>
       </c>
       <c r="G205" s="6" t="s">
         <v>522</v>
@@ -10372,7 +10381,7 @@
         <v>483</v>
       </c>
       <c r="F206" s="3" t="s">
-        <v>923</v>
+        <v>941</v>
       </c>
       <c r="G206" s="6" t="s">
         <v>522</v>
@@ -10392,7 +10401,7 @@
         <v>488</v>
       </c>
       <c r="F207" s="3" t="s">
-        <v>923</v>
+        <v>941</v>
       </c>
       <c r="G207" s="6" t="s">
         <v>522</v>
@@ -10412,7 +10421,7 @@
         <v>493</v>
       </c>
       <c r="F208" s="3" t="s">
-        <v>923</v>
+        <v>941</v>
       </c>
       <c r="G208" s="6" t="s">
         <v>522</v>
@@ -10432,7 +10441,7 @@
         <v>498</v>
       </c>
       <c r="F209" s="3" t="s">
-        <v>923</v>
+        <v>941</v>
       </c>
       <c r="G209" s="6" t="s">
         <v>522</v>
@@ -10452,7 +10461,7 @@
         <v>503</v>
       </c>
       <c r="F210" s="3" t="s">
-        <v>923</v>
+        <v>941</v>
       </c>
       <c r="G210" s="6" t="s">
         <v>522</v>
@@ -10472,7 +10481,7 @@
         <v>508</v>
       </c>
       <c r="F211" s="3" t="s">
-        <v>923</v>
+        <v>941</v>
       </c>
       <c r="G211" s="6" t="s">
         <v>522</v>
@@ -10492,7 +10501,7 @@
         <v>513</v>
       </c>
       <c r="F212" s="3" t="s">
-        <v>923</v>
+        <v>941</v>
       </c>
       <c r="G212" s="6" t="s">
         <v>522</v>
@@ -10512,7 +10521,7 @@
         <v>518</v>
       </c>
       <c r="F213" s="3" t="s">
-        <v>923</v>
+        <v>941</v>
       </c>
       <c r="G213" s="6" t="s">
         <v>522</v>
@@ -10532,7 +10541,7 @@
         <v>888</v>
       </c>
       <c r="F214" s="3" t="s">
-        <v>923</v>
+        <v>941</v>
       </c>
       <c r="G214" s="6" t="s">
         <v>522</v>
@@ -10552,7 +10561,7 @@
         <v>444</v>
       </c>
       <c r="F215" s="3" t="s">
-        <v>923</v>
+        <v>941</v>
       </c>
       <c r="G215" s="6" t="s">
         <v>522</v>
@@ -10572,7 +10581,7 @@
         <v>449</v>
       </c>
       <c r="F216" s="3" t="s">
-        <v>923</v>
+        <v>941</v>
       </c>
       <c r="G216" s="6" t="s">
         <v>522</v>
@@ -10592,7 +10601,7 @@
         <v>454</v>
       </c>
       <c r="F217" s="3" t="s">
-        <v>923</v>
+        <v>941</v>
       </c>
       <c r="G217" s="6" t="s">
         <v>522</v>
@@ -10612,7 +10621,7 @@
         <v>459</v>
       </c>
       <c r="F218" s="3" t="s">
-        <v>923</v>
+        <v>941</v>
       </c>
       <c r="G218" s="6" t="s">
         <v>522</v>
@@ -10632,7 +10641,7 @@
         <v>464</v>
       </c>
       <c r="F219" s="3" t="s">
-        <v>923</v>
+        <v>941</v>
       </c>
       <c r="G219" s="6" t="s">
         <v>522</v>
@@ -10652,7 +10661,7 @@
         <v>469</v>
       </c>
       <c r="F220" s="3" t="s">
-        <v>923</v>
+        <v>941</v>
       </c>
       <c r="G220" s="6" t="s">
         <v>522</v>
@@ -10672,7 +10681,7 @@
         <v>474</v>
       </c>
       <c r="F221" s="3" t="s">
-        <v>923</v>
+        <v>941</v>
       </c>
       <c r="G221" s="6" t="s">
         <v>522</v>
@@ -10692,7 +10701,7 @@
         <v>479</v>
       </c>
       <c r="F222" s="3" t="s">
-        <v>923</v>
+        <v>941</v>
       </c>
       <c r="G222" s="6" t="s">
         <v>522</v>
@@ -10712,7 +10721,7 @@
         <v>484</v>
       </c>
       <c r="F223" s="3" t="s">
-        <v>923</v>
+        <v>941</v>
       </c>
       <c r="G223" s="6" t="s">
         <v>522</v>
@@ -10732,7 +10741,7 @@
         <v>489</v>
       </c>
       <c r="F224" s="3" t="s">
-        <v>923</v>
+        <v>941</v>
       </c>
       <c r="G224" s="6" t="s">
         <v>522</v>
@@ -10752,7 +10761,7 @@
         <v>494</v>
       </c>
       <c r="F225" s="3" t="s">
-        <v>923</v>
+        <v>941</v>
       </c>
       <c r="G225" s="6" t="s">
         <v>522</v>
@@ -10772,7 +10781,7 @@
         <v>499</v>
       </c>
       <c r="F226" s="3" t="s">
-        <v>923</v>
+        <v>941</v>
       </c>
       <c r="G226" s="6" t="s">
         <v>522</v>
@@ -10792,7 +10801,7 @@
         <v>504</v>
       </c>
       <c r="F227" s="3" t="s">
-        <v>923</v>
+        <v>941</v>
       </c>
       <c r="G227" s="6" t="s">
         <v>522</v>
@@ -10812,7 +10821,7 @@
         <v>509</v>
       </c>
       <c r="F228" s="3" t="s">
-        <v>923</v>
+        <v>941</v>
       </c>
       <c r="G228" s="6" t="s">
         <v>522</v>
@@ -10832,7 +10841,7 @@
         <v>514</v>
       </c>
       <c r="F229" s="3" t="s">
-        <v>923</v>
+        <v>941</v>
       </c>
       <c r="G229" s="6" t="s">
         <v>522</v>
@@ -10852,7 +10861,7 @@
         <v>519</v>
       </c>
       <c r="F230" s="3" t="s">
-        <v>923</v>
+        <v>941</v>
       </c>
       <c r="G230" s="6" t="s">
         <v>522</v>
@@ -10872,7 +10881,7 @@
         <v>889</v>
       </c>
       <c r="F231" s="3" t="s">
-        <v>923</v>
+        <v>941</v>
       </c>
       <c r="G231" s="6" t="s">
         <v>522</v>
@@ -10892,7 +10901,7 @@
         <v>445</v>
       </c>
       <c r="F232" s="3" t="s">
-        <v>923</v>
+        <v>941</v>
       </c>
       <c r="G232" s="6" t="s">
         <v>522</v>
@@ -10912,7 +10921,7 @@
         <v>450</v>
       </c>
       <c r="F233" s="3" t="s">
-        <v>923</v>
+        <v>941</v>
       </c>
       <c r="G233" s="6" t="s">
         <v>522</v>
@@ -10932,7 +10941,7 @@
         <v>455</v>
       </c>
       <c r="F234" s="3" t="s">
-        <v>923</v>
+        <v>941</v>
       </c>
       <c r="G234" s="6" t="s">
         <v>522</v>
@@ -10952,7 +10961,7 @@
         <v>460</v>
       </c>
       <c r="F235" s="3" t="s">
-        <v>923</v>
+        <v>941</v>
       </c>
       <c r="G235" s="6" t="s">
         <v>522</v>
@@ -10972,7 +10981,7 @@
         <v>465</v>
       </c>
       <c r="F236" s="3" t="s">
-        <v>923</v>
+        <v>941</v>
       </c>
       <c r="G236" s="6" t="s">
         <v>522</v>
@@ -10992,7 +11001,7 @@
         <v>470</v>
       </c>
       <c r="F237" s="3" t="s">
-        <v>923</v>
+        <v>941</v>
       </c>
       <c r="G237" s="6" t="s">
         <v>522</v>
@@ -11012,7 +11021,7 @@
         <v>475</v>
       </c>
       <c r="F238" s="3" t="s">
-        <v>923</v>
+        <v>941</v>
       </c>
       <c r="G238" s="6" t="s">
         <v>522</v>
@@ -11032,7 +11041,7 @@
         <v>480</v>
       </c>
       <c r="F239" s="3" t="s">
-        <v>923</v>
+        <v>941</v>
       </c>
       <c r="G239" s="6" t="s">
         <v>522</v>
@@ -11052,7 +11061,7 @@
         <v>485</v>
       </c>
       <c r="F240" s="3" t="s">
-        <v>923</v>
+        <v>941</v>
       </c>
       <c r="G240" s="6" t="s">
         <v>522</v>
@@ -11072,7 +11081,7 @@
         <v>490</v>
       </c>
       <c r="F241" s="3" t="s">
-        <v>923</v>
+        <v>941</v>
       </c>
       <c r="G241" s="6" t="s">
         <v>522</v>
@@ -11092,7 +11101,7 @@
         <v>495</v>
       </c>
       <c r="F242" s="3" t="s">
-        <v>923</v>
+        <v>941</v>
       </c>
       <c r="G242" s="6" t="s">
         <v>522</v>
@@ -11112,7 +11121,7 @@
         <v>500</v>
       </c>
       <c r="F243" s="3" t="s">
-        <v>923</v>
+        <v>941</v>
       </c>
       <c r="G243" s="6" t="s">
         <v>522</v>
@@ -11132,7 +11141,7 @@
         <v>505</v>
       </c>
       <c r="F244" s="3" t="s">
-        <v>923</v>
+        <v>941</v>
       </c>
       <c r="G244" s="6" t="s">
         <v>522</v>
@@ -11152,7 +11161,7 @@
         <v>510</v>
       </c>
       <c r="F245" s="3" t="s">
-        <v>923</v>
+        <v>941</v>
       </c>
       <c r="G245" s="6" t="s">
         <v>522</v>
@@ -11172,7 +11181,7 @@
         <v>515</v>
       </c>
       <c r="F246" s="3" t="s">
-        <v>923</v>
+        <v>941</v>
       </c>
       <c r="G246" s="6" t="s">
         <v>522</v>
@@ -11192,7 +11201,7 @@
         <v>520</v>
       </c>
       <c r="F247" s="3" t="s">
-        <v>923</v>
+        <v>941</v>
       </c>
       <c r="G247" s="6" t="s">
         <v>522</v>
@@ -11212,7 +11221,7 @@
         <v>441</v>
       </c>
       <c r="F248" s="3" t="s">
-        <v>923</v>
+        <v>941</v>
       </c>
       <c r="G248" s="6" t="s">
         <v>522</v>
@@ -11232,7 +11241,7 @@
         <v>446</v>
       </c>
       <c r="F249" s="3" t="s">
-        <v>923</v>
+        <v>941</v>
       </c>
       <c r="G249" s="6" t="s">
         <v>522</v>
@@ -11252,7 +11261,7 @@
         <v>451</v>
       </c>
       <c r="F250" s="3" t="s">
-        <v>923</v>
+        <v>941</v>
       </c>
       <c r="G250" s="6" t="s">
         <v>522</v>
@@ -11272,7 +11281,7 @@
         <v>456</v>
       </c>
       <c r="F251" s="3" t="s">
-        <v>923</v>
+        <v>941</v>
       </c>
       <c r="G251" s="6" t="s">
         <v>522</v>
@@ -11292,7 +11301,7 @@
         <v>461</v>
       </c>
       <c r="F252" s="3" t="s">
-        <v>923</v>
+        <v>941</v>
       </c>
       <c r="G252" s="6" t="s">
         <v>522</v>
@@ -11312,7 +11321,7 @@
         <v>466</v>
       </c>
       <c r="F253" s="3" t="s">
-        <v>923</v>
+        <v>941</v>
       </c>
       <c r="G253" s="6" t="s">
         <v>522</v>
@@ -11332,7 +11341,7 @@
         <v>471</v>
       </c>
       <c r="F254" s="3" t="s">
-        <v>923</v>
+        <v>941</v>
       </c>
       <c r="G254" s="6" t="s">
         <v>522</v>
@@ -11352,7 +11361,7 @@
         <v>476</v>
       </c>
       <c r="F255" s="3" t="s">
-        <v>923</v>
+        <v>941</v>
       </c>
       <c r="G255" s="6" t="s">
         <v>522</v>
@@ -11372,7 +11381,7 @@
         <v>481</v>
       </c>
       <c r="F256" s="3" t="s">
-        <v>923</v>
+        <v>941</v>
       </c>
       <c r="G256" s="6" t="s">
         <v>522</v>
@@ -11392,7 +11401,7 @@
         <v>486</v>
       </c>
       <c r="F257" s="3" t="s">
-        <v>923</v>
+        <v>941</v>
       </c>
       <c r="G257" s="6" t="s">
         <v>522</v>
@@ -11412,7 +11421,7 @@
         <v>491</v>
       </c>
       <c r="F258" s="3" t="s">
-        <v>923</v>
+        <v>941</v>
       </c>
       <c r="G258" s="6" t="s">
         <v>522</v>
@@ -11432,7 +11441,7 @@
         <v>496</v>
       </c>
       <c r="F259" s="3" t="s">
-        <v>923</v>
+        <v>941</v>
       </c>
       <c r="G259" s="6" t="s">
         <v>522</v>
@@ -11452,7 +11461,7 @@
         <v>501</v>
       </c>
       <c r="F260" s="3" t="s">
-        <v>923</v>
+        <v>941</v>
       </c>
       <c r="G260" s="6" t="s">
         <v>522</v>
@@ -11472,7 +11481,7 @@
         <v>506</v>
       </c>
       <c r="F261" s="3" t="s">
-        <v>923</v>
+        <v>941</v>
       </c>
       <c r="G261" s="6" t="s">
         <v>522</v>
@@ -11492,7 +11501,7 @@
         <v>511</v>
       </c>
       <c r="F262" s="3" t="s">
-        <v>923</v>
+        <v>941</v>
       </c>
       <c r="G262" s="6" t="s">
         <v>522</v>
@@ -11512,7 +11521,7 @@
         <v>516</v>
       </c>
       <c r="F263" s="3" t="s">
-        <v>923</v>
+        <v>941</v>
       </c>
       <c r="G263" s="6" t="s">
         <v>522</v>
@@ -11532,7 +11541,7 @@
         <v>442</v>
       </c>
       <c r="F264" s="3" t="s">
-        <v>923</v>
+        <v>941</v>
       </c>
       <c r="G264" s="6" t="s">
         <v>522</v>
@@ -11552,7 +11561,7 @@
         <v>447</v>
       </c>
       <c r="F265" s="3" t="s">
-        <v>923</v>
+        <v>941</v>
       </c>
       <c r="G265" s="6" t="s">
         <v>522</v>
@@ -11572,7 +11581,7 @@
         <v>452</v>
       </c>
       <c r="F266" s="3" t="s">
-        <v>923</v>
+        <v>941</v>
       </c>
       <c r="G266" s="6" t="s">
         <v>522</v>
@@ -11592,7 +11601,7 @@
         <v>457</v>
       </c>
       <c r="F267" s="3" t="s">
-        <v>923</v>
+        <v>941</v>
       </c>
       <c r="G267" s="6" t="s">
         <v>522</v>
@@ -11612,7 +11621,7 @@
         <v>462</v>
       </c>
       <c r="F268" s="3" t="s">
-        <v>923</v>
+        <v>941</v>
       </c>
       <c r="G268" s="6" t="s">
         <v>522</v>
@@ -11632,7 +11641,7 @@
         <v>467</v>
       </c>
       <c r="F269" s="3" t="s">
-        <v>923</v>
+        <v>941</v>
       </c>
       <c r="G269" s="6" t="s">
         <v>522</v>
@@ -11652,7 +11661,7 @@
         <v>472</v>
       </c>
       <c r="F270" s="3" t="s">
-        <v>923</v>
+        <v>941</v>
       </c>
       <c r="G270" s="6" t="s">
         <v>522</v>
@@ -11672,7 +11681,7 @@
         <v>477</v>
       </c>
       <c r="F271" s="3" t="s">
-        <v>923</v>
+        <v>941</v>
       </c>
       <c r="G271" s="6" t="s">
         <v>522</v>
@@ -11692,7 +11701,7 @@
         <v>482</v>
       </c>
       <c r="F272" s="3" t="s">
-        <v>923</v>
+        <v>941</v>
       </c>
       <c r="G272" s="6" t="s">
         <v>522</v>
@@ -11712,7 +11721,7 @@
         <v>487</v>
       </c>
       <c r="F273" s="3" t="s">
-        <v>923</v>
+        <v>941</v>
       </c>
       <c r="G273" s="6" t="s">
         <v>522</v>
@@ -11732,7 +11741,7 @@
         <v>492</v>
       </c>
       <c r="F274" s="3" t="s">
-        <v>923</v>
+        <v>941</v>
       </c>
       <c r="G274" s="6" t="s">
         <v>522</v>
@@ -11752,7 +11761,7 @@
         <v>497</v>
       </c>
       <c r="F275" s="3" t="s">
-        <v>923</v>
+        <v>941</v>
       </c>
       <c r="G275" s="6" t="s">
         <v>522</v>
@@ -11772,7 +11781,7 @@
         <v>502</v>
       </c>
       <c r="F276" s="3" t="s">
-        <v>923</v>
+        <v>941</v>
       </c>
       <c r="G276" s="6" t="s">
         <v>522</v>
@@ -11792,7 +11801,7 @@
         <v>507</v>
       </c>
       <c r="F277" s="3" t="s">
-        <v>923</v>
+        <v>941</v>
       </c>
       <c r="G277" s="6" t="s">
         <v>522</v>
@@ -11812,7 +11821,7 @@
         <v>512</v>
       </c>
       <c r="F278" s="3" t="s">
-        <v>923</v>
+        <v>941</v>
       </c>
       <c r="G278" s="6" t="s">
         <v>522</v>
@@ -11832,7 +11841,7 @@
         <v>517</v>
       </c>
       <c r="F279" s="3" t="s">
-        <v>923</v>
+        <v>941</v>
       </c>
       <c r="G279" s="6" t="s">
         <v>522</v>
@@ -11852,7 +11861,7 @@
         <v>809</v>
       </c>
       <c r="F280" s="3" t="s">
-        <v>923</v>
+        <v>942</v>
       </c>
       <c r="G280" s="6" t="s">
         <v>525</v>
@@ -11872,7 +11881,7 @@
         <v>810</v>
       </c>
       <c r="F281" s="3" t="s">
-        <v>923</v>
+        <v>942</v>
       </c>
       <c r="G281" s="6" t="s">
         <v>525</v>
@@ -11892,7 +11901,7 @@
         <v>808</v>
       </c>
       <c r="F282" s="3" t="s">
-        <v>923</v>
+        <v>942</v>
       </c>
       <c r="G282" s="6" t="s">
         <v>525</v>
@@ -11912,7 +11921,7 @@
         <v>811</v>
       </c>
       <c r="F283" s="3" t="s">
-        <v>923</v>
+        <v>942</v>
       </c>
       <c r="G283" s="6" t="s">
         <v>525</v>
@@ -11932,7 +11941,7 @@
         <v>812</v>
       </c>
       <c r="F284" s="3" t="s">
-        <v>923</v>
+        <v>942</v>
       </c>
       <c r="G284" s="6" t="s">
         <v>525</v>
@@ -11952,7 +11961,7 @@
         <v>813</v>
       </c>
       <c r="F285" s="3" t="s">
-        <v>923</v>
+        <v>942</v>
       </c>
       <c r="G285" s="6" t="s">
         <v>525</v>
@@ -11972,7 +11981,7 @@
         <v>814</v>
       </c>
       <c r="F286" s="3" t="s">
-        <v>923</v>
+        <v>942</v>
       </c>
       <c r="G286" s="6" t="s">
         <v>525</v>
@@ -11992,7 +12001,7 @@
         <v>815</v>
       </c>
       <c r="F287" s="3" t="s">
-        <v>923</v>
+        <v>942</v>
       </c>
       <c r="G287" s="6" t="s">
         <v>525</v>
@@ -13199,7 +13208,7 @@
         <v>885</v>
       </c>
       <c r="F358" s="3" t="s">
-        <v>923</v>
+        <v>943</v>
       </c>
       <c r="G358" s="3" t="s">
         <v>250</v>
@@ -13216,7 +13225,7 @@
         <v>887</v>
       </c>
       <c r="F359" s="3" t="s">
-        <v>923</v>
+        <v>943</v>
       </c>
       <c r="G359" s="3" t="s">
         <v>250</v>
@@ -13233,7 +13242,7 @@
         <v>626</v>
       </c>
       <c r="F360" s="3" t="s">
-        <v>923</v>
+        <v>942</v>
       </c>
       <c r="G360" s="3" t="s">
         <v>886</v>
@@ -13250,7 +13259,7 @@
         <v>627</v>
       </c>
       <c r="F361" s="3" t="s">
-        <v>923</v>
+        <v>942</v>
       </c>
       <c r="G361" s="3" t="s">
         <v>886</v>
@@ -13267,7 +13276,7 @@
         <v>628</v>
       </c>
       <c r="F362" s="3" t="s">
-        <v>923</v>
+        <v>942</v>
       </c>
       <c r="G362" s="3" t="s">
         <v>886</v>
@@ -13284,7 +13293,7 @@
         <v>629</v>
       </c>
       <c r="F363" s="3" t="s">
-        <v>923</v>
+        <v>942</v>
       </c>
       <c r="G363" s="3" t="s">
         <v>886</v>
@@ -13301,7 +13310,7 @@
         <v>630</v>
       </c>
       <c r="F364" s="3" t="s">
-        <v>923</v>
+        <v>942</v>
       </c>
       <c r="G364" s="3" t="s">
         <v>886</v>
@@ -13318,7 +13327,7 @@
         <v>631</v>
       </c>
       <c r="F365" s="3" t="s">
-        <v>923</v>
+        <v>942</v>
       </c>
       <c r="G365" s="3" t="s">
         <v>886</v>
@@ -13335,7 +13344,7 @@
         <v>632</v>
       </c>
       <c r="F366" s="3" t="s">
-        <v>923</v>
+        <v>942</v>
       </c>
       <c r="G366" s="3" t="s">
         <v>886</v>
@@ -13352,7 +13361,7 @@
         <v>633</v>
       </c>
       <c r="F367" s="3" t="s">
-        <v>923</v>
+        <v>942</v>
       </c>
       <c r="G367" s="3" t="s">
         <v>886</v>
@@ -13369,7 +13378,7 @@
         <v>634</v>
       </c>
       <c r="F368" s="3" t="s">
-        <v>923</v>
+        <v>942</v>
       </c>
       <c r="G368" s="3" t="s">
         <v>886</v>
@@ -13386,7 +13395,7 @@
         <v>635</v>
       </c>
       <c r="F369" s="3" t="s">
-        <v>923</v>
+        <v>942</v>
       </c>
       <c r="G369" s="3" t="s">
         <v>886</v>
@@ -13403,7 +13412,7 @@
         <v>636</v>
       </c>
       <c r="F370" s="3" t="s">
-        <v>923</v>
+        <v>942</v>
       </c>
       <c r="G370" s="3" t="s">
         <v>886</v>
@@ -13420,7 +13429,7 @@
         <v>637</v>
       </c>
       <c r="F371" s="3" t="s">
-        <v>923</v>
+        <v>942</v>
       </c>
       <c r="G371" s="3" t="s">
         <v>886</v>
@@ -13437,7 +13446,7 @@
         <v>638</v>
       </c>
       <c r="F372" s="3" t="s">
-        <v>923</v>
+        <v>942</v>
       </c>
       <c r="G372" s="3" t="s">
         <v>886</v>
@@ -13454,7 +13463,7 @@
         <v>639</v>
       </c>
       <c r="F373" s="3" t="s">
-        <v>923</v>
+        <v>942</v>
       </c>
       <c r="G373" s="3" t="s">
         <v>886</v>
@@ -13471,7 +13480,7 @@
         <v>640</v>
       </c>
       <c r="F374" s="3" t="s">
-        <v>923</v>
+        <v>942</v>
       </c>
       <c r="G374" s="3" t="s">
         <v>886</v>
@@ -13488,7 +13497,7 @@
         <v>641</v>
       </c>
       <c r="F375" s="3" t="s">
-        <v>923</v>
+        <v>942</v>
       </c>
       <c r="G375" s="3" t="s">
         <v>886</v>
@@ -13505,7 +13514,7 @@
         <v>642</v>
       </c>
       <c r="F376" s="3" t="s">
-        <v>923</v>
+        <v>942</v>
       </c>
       <c r="G376" s="3" t="s">
         <v>886</v>
@@ -13522,7 +13531,7 @@
         <v>643</v>
       </c>
       <c r="F377" s="3" t="s">
-        <v>923</v>
+        <v>942</v>
       </c>
       <c r="G377" s="3" t="s">
         <v>886</v>
@@ -13539,7 +13548,7 @@
         <v>644</v>
       </c>
       <c r="F378" s="3" t="s">
-        <v>923</v>
+        <v>942</v>
       </c>
       <c r="G378" s="3" t="s">
         <v>886</v>
@@ -13556,7 +13565,7 @@
         <v>645</v>
       </c>
       <c r="F379" s="3" t="s">
-        <v>923</v>
+        <v>942</v>
       </c>
       <c r="G379" s="3" t="s">
         <v>886</v>
@@ -13573,7 +13582,7 @@
         <v>646</v>
       </c>
       <c r="F380" s="3" t="s">
-        <v>923</v>
+        <v>942</v>
       </c>
       <c r="G380" s="3" t="s">
         <v>886</v>
@@ -13590,7 +13599,7 @@
         <v>647</v>
       </c>
       <c r="F381" s="3" t="s">
-        <v>923</v>
+        <v>942</v>
       </c>
       <c r="G381" s="3" t="s">
         <v>886</v>
@@ -13607,7 +13616,7 @@
         <v>648</v>
       </c>
       <c r="F382" s="3" t="s">
-        <v>923</v>
+        <v>942</v>
       </c>
       <c r="G382" s="3" t="s">
         <v>886</v>
@@ -13624,7 +13633,7 @@
         <v>649</v>
       </c>
       <c r="F383" s="3" t="s">
-        <v>923</v>
+        <v>942</v>
       </c>
       <c r="G383" s="3" t="s">
         <v>886</v>
@@ -13641,7 +13650,7 @@
         <v>650</v>
       </c>
       <c r="F384" s="3" t="s">
-        <v>923</v>
+        <v>942</v>
       </c>
       <c r="G384" s="3" t="s">
         <v>886</v>
@@ -13658,7 +13667,7 @@
         <v>651</v>
       </c>
       <c r="F385" s="3" t="s">
-        <v>923</v>
+        <v>942</v>
       </c>
       <c r="G385" s="3" t="s">
         <v>886</v>
@@ -13675,7 +13684,7 @@
         <v>652</v>
       </c>
       <c r="F386" s="3" t="s">
-        <v>923</v>
+        <v>942</v>
       </c>
       <c r="G386" s="3" t="s">
         <v>886</v>
@@ -13692,7 +13701,7 @@
         <v>653</v>
       </c>
       <c r="F387" s="3" t="s">
-        <v>923</v>
+        <v>942</v>
       </c>
       <c r="G387" s="3" t="s">
         <v>886</v>
@@ -13709,7 +13718,7 @@
         <v>654</v>
       </c>
       <c r="F388" s="3" t="s">
-        <v>923</v>
+        <v>942</v>
       </c>
       <c r="G388" s="3" t="s">
         <v>886</v>
@@ -13726,7 +13735,7 @@
         <v>655</v>
       </c>
       <c r="F389" s="3" t="s">
-        <v>923</v>
+        <v>942</v>
       </c>
       <c r="G389" s="3" t="s">
         <v>886</v>
@@ -13743,7 +13752,7 @@
         <v>656</v>
       </c>
       <c r="F390" s="3" t="s">
-        <v>923</v>
+        <v>942</v>
       </c>
       <c r="G390" s="3" t="s">
         <v>886</v>
@@ -13760,7 +13769,7 @@
         <v>657</v>
       </c>
       <c r="F391" s="3" t="s">
-        <v>923</v>
+        <v>942</v>
       </c>
       <c r="G391" s="3" t="s">
         <v>886</v>
@@ -13777,7 +13786,7 @@
         <v>658</v>
       </c>
       <c r="F392" s="3" t="s">
-        <v>923</v>
+        <v>942</v>
       </c>
       <c r="G392" s="3" t="s">
         <v>886</v>
@@ -13794,7 +13803,7 @@
         <v>659</v>
       </c>
       <c r="F393" s="3" t="s">
-        <v>923</v>
+        <v>942</v>
       </c>
       <c r="G393" s="3" t="s">
         <v>886</v>
@@ -13811,7 +13820,7 @@
         <v>660</v>
       </c>
       <c r="F394" s="3" t="s">
-        <v>923</v>
+        <v>942</v>
       </c>
       <c r="G394" s="3" t="s">
         <v>886</v>
@@ -13828,7 +13837,7 @@
         <v>661</v>
       </c>
       <c r="F395" s="3" t="s">
-        <v>923</v>
+        <v>942</v>
       </c>
       <c r="G395" s="3" t="s">
         <v>886</v>
@@ -13845,7 +13854,7 @@
         <v>662</v>
       </c>
       <c r="F396" s="3" t="s">
-        <v>923</v>
+        <v>942</v>
       </c>
       <c r="G396" s="3" t="s">
         <v>886</v>
@@ -13862,7 +13871,7 @@
         <v>663</v>
       </c>
       <c r="F397" s="3" t="s">
-        <v>923</v>
+        <v>942</v>
       </c>
       <c r="G397" s="3" t="s">
         <v>886</v>
@@ -13879,7 +13888,7 @@
         <v>664</v>
       </c>
       <c r="F398" s="3" t="s">
-        <v>923</v>
+        <v>942</v>
       </c>
       <c r="G398" s="3" t="s">
         <v>886</v>
@@ -13896,7 +13905,7 @@
         <v>665</v>
       </c>
       <c r="F399" s="3" t="s">
-        <v>923</v>
+        <v>942</v>
       </c>
       <c r="G399" s="3" t="s">
         <v>886</v>
@@ -13913,7 +13922,7 @@
         <v>666</v>
       </c>
       <c r="F400" s="3" t="s">
-        <v>923</v>
+        <v>942</v>
       </c>
       <c r="G400" s="3" t="s">
         <v>886</v>
@@ -13930,7 +13939,7 @@
         <v>667</v>
       </c>
       <c r="F401" s="3" t="s">
-        <v>923</v>
+        <v>942</v>
       </c>
       <c r="G401" s="3" t="s">
         <v>886</v>
@@ -13947,7 +13956,7 @@
         <v>668</v>
       </c>
       <c r="F402" s="3" t="s">
-        <v>923</v>
+        <v>942</v>
       </c>
       <c r="G402" s="3" t="s">
         <v>886</v>
@@ -13964,7 +13973,7 @@
         <v>669</v>
       </c>
       <c r="F403" s="3" t="s">
-        <v>923</v>
+        <v>942</v>
       </c>
       <c r="G403" s="3" t="s">
         <v>886</v>
@@ -13981,7 +13990,7 @@
         <v>670</v>
       </c>
       <c r="F404" s="3" t="s">
-        <v>923</v>
+        <v>942</v>
       </c>
       <c r="G404" s="3" t="s">
         <v>886</v>
@@ -13998,7 +14007,7 @@
         <v>671</v>
       </c>
       <c r="F405" s="3" t="s">
-        <v>923</v>
+        <v>942</v>
       </c>
       <c r="G405" s="3" t="s">
         <v>886</v>
@@ -14015,7 +14024,7 @@
         <v>672</v>
       </c>
       <c r="F406" s="3" t="s">
-        <v>923</v>
+        <v>942</v>
       </c>
       <c r="G406" s="3" t="s">
         <v>886</v>
@@ -14032,7 +14041,7 @@
         <v>673</v>
       </c>
       <c r="F407" s="3" t="s">
-        <v>923</v>
+        <v>942</v>
       </c>
       <c r="G407" s="3" t="s">
         <v>886</v>
@@ -14049,7 +14058,7 @@
         <v>674</v>
       </c>
       <c r="F408" s="3" t="s">
-        <v>923</v>
+        <v>942</v>
       </c>
       <c r="G408" s="3" t="s">
         <v>886</v>
@@ -14066,7 +14075,7 @@
         <v>675</v>
       </c>
       <c r="F409" s="3" t="s">
-        <v>923</v>
+        <v>942</v>
       </c>
       <c r="G409" s="3" t="s">
         <v>886</v>
@@ -14083,7 +14092,7 @@
         <v>676</v>
       </c>
       <c r="F410" s="3" t="s">
-        <v>923</v>
+        <v>942</v>
       </c>
       <c r="G410" s="3" t="s">
         <v>886</v>
@@ -14100,7 +14109,7 @@
         <v>677</v>
       </c>
       <c r="F411" s="3" t="s">
-        <v>923</v>
+        <v>942</v>
       </c>
       <c r="G411" s="3" t="s">
         <v>886</v>
@@ -14117,7 +14126,7 @@
         <v>678</v>
       </c>
       <c r="F412" s="3" t="s">
-        <v>923</v>
+        <v>942</v>
       </c>
       <c r="G412" s="3" t="s">
         <v>886</v>
@@ -14134,7 +14143,7 @@
         <v>679</v>
       </c>
       <c r="F413" s="3" t="s">
-        <v>923</v>
+        <v>942</v>
       </c>
       <c r="G413" s="3" t="s">
         <v>886</v>
@@ -14151,7 +14160,7 @@
         <v>680</v>
       </c>
       <c r="F414" s="3" t="s">
-        <v>923</v>
+        <v>942</v>
       </c>
       <c r="G414" s="3" t="s">
         <v>886</v>
@@ -14168,7 +14177,7 @@
         <v>681</v>
       </c>
       <c r="F415" s="3" t="s">
-        <v>923</v>
+        <v>942</v>
       </c>
       <c r="G415" s="3" t="s">
         <v>886</v>
@@ -14185,7 +14194,7 @@
         <v>682</v>
       </c>
       <c r="F416" s="3" t="s">
-        <v>923</v>
+        <v>942</v>
       </c>
       <c r="G416" s="3" t="s">
         <v>886</v>
@@ -14202,7 +14211,7 @@
         <v>683</v>
       </c>
       <c r="F417" s="3" t="s">
-        <v>923</v>
+        <v>942</v>
       </c>
       <c r="G417" s="3" t="s">
         <v>886</v>
@@ -14219,7 +14228,7 @@
         <v>684</v>
       </c>
       <c r="F418" s="3" t="s">
-        <v>923</v>
+        <v>942</v>
       </c>
       <c r="G418" s="3" t="s">
         <v>886</v>
@@ -14236,7 +14245,7 @@
         <v>685</v>
       </c>
       <c r="F419" s="3" t="s">
-        <v>923</v>
+        <v>942</v>
       </c>
       <c r="G419" s="3" t="s">
         <v>886</v>
@@ -14247,16 +14256,16 @@
     </row>
     <row r="420" spans="2:10" ht="14" x14ac:dyDescent="0.15">
       <c r="B420" s="6" t="s">
+        <v>929</v>
+      </c>
+      <c r="C420" s="6" t="s">
         <v>930</v>
       </c>
-      <c r="C420" s="6" t="s">
-        <v>931</v>
-      </c>
       <c r="F420" s="6" t="s">
-        <v>928</v>
+        <v>927</v>
       </c>
       <c r="G420" s="6" t="s">
-        <v>928</v>
+        <v>927</v>
       </c>
       <c r="J420" s="6" t="s">
         <v>254</v>
@@ -14264,16 +14273,16 @@
     </row>
     <row r="421" spans="2:10" ht="14" x14ac:dyDescent="0.15">
       <c r="B421" s="6" t="s">
-        <v>941</v>
+        <v>940</v>
       </c>
       <c r="C421" s="6" t="s">
-        <v>932</v>
+        <v>931</v>
       </c>
       <c r="F421" s="6" t="s">
-        <v>928</v>
+        <v>927</v>
       </c>
       <c r="G421" s="6" t="s">
-        <v>928</v>
+        <v>927</v>
       </c>
       <c r="J421" s="6" t="s">
         <v>254</v>
@@ -14281,10 +14290,10 @@
     </row>
     <row r="422" spans="2:10" ht="14" x14ac:dyDescent="0.15">
       <c r="B422" s="6" t="s">
+        <v>932</v>
+      </c>
+      <c r="C422" s="6" t="s">
         <v>933</v>
-      </c>
-      <c r="C422" s="6" t="s">
-        <v>934</v>
       </c>
       <c r="F422" s="2" t="s">
         <v>48</v>
@@ -14298,13 +14307,13 @@
     </row>
     <row r="423" spans="2:10" ht="14" x14ac:dyDescent="0.15">
       <c r="B423" s="6" t="s">
-        <v>935</v>
+        <v>934</v>
       </c>
       <c r="C423" s="6" t="s">
-        <v>938</v>
+        <v>937</v>
       </c>
       <c r="F423" s="3" t="s">
-        <v>923</v>
+        <v>943</v>
       </c>
       <c r="G423" s="3" t="s">
         <v>923</v>
@@ -14315,13 +14324,13 @@
     </row>
     <row r="424" spans="2:10" ht="14" x14ac:dyDescent="0.15">
       <c r="B424" s="6" t="s">
-        <v>936</v>
+        <v>935</v>
       </c>
       <c r="C424" s="6" t="s">
-        <v>939</v>
+        <v>938</v>
       </c>
       <c r="F424" s="3" t="s">
-        <v>923</v>
+        <v>943</v>
       </c>
       <c r="G424" s="3" t="s">
         <v>923</v>
@@ -14332,13 +14341,13 @@
     </row>
     <row r="425" spans="2:10" ht="14" x14ac:dyDescent="0.15">
       <c r="B425" s="6" t="s">
-        <v>937</v>
+        <v>936</v>
       </c>
       <c r="C425" s="6" t="s">
-        <v>940</v>
+        <v>939</v>
       </c>
       <c r="F425" s="3" t="s">
-        <v>923</v>
+        <v>943</v>
       </c>
       <c r="G425" s="3" t="s">
         <v>923</v>

</xml_diff>

<commit_message>
Updating nice labels to data dictionary.
</commit_message>
<xml_diff>
--- a/data/processed/Data_Dictionary.xlsx
+++ b/data/processed/Data_Dictionary.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/davidmccoy/COVIDxrisk/data/processed/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{78C8CAB3-5694-B440-A73E-748BEB5774D8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D2BE6332-E36C-3543-B0C0-8B6E13B854E6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="30440" yWindow="500" windowWidth="48940" windowHeight="25540" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3132" uniqueCount="946">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3196" uniqueCount="1010">
   <si>
     <t>Col Num</t>
   </si>
@@ -2996,6 +2996,198 @@
   </si>
   <si>
     <t>occ_educ_health</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Proportion White  </t>
+  </si>
+  <si>
+    <t>All Heart Disease Death Rate</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Poor or Fair Health </t>
+  </si>
+  <si>
+    <t>Poor Physical Health Days</t>
+  </si>
+  <si>
+    <t>Limited Access to Healthy Foods</t>
+  </si>
+  <si>
+    <t>Prevalence of Alcohol Abuse</t>
+  </si>
+  <si>
+    <t>Prevalance with Atrial Fibrillation</t>
+  </si>
+  <si>
+    <t>Prevalence with Heart Failure</t>
+  </si>
+  <si>
+    <t>Prevalance Stroke</t>
+  </si>
+  <si>
+    <t>Prevalence under 65 of Alcohol Abuse</t>
+  </si>
+  <si>
+    <t>Prevalence under 65 Arthritis</t>
+  </si>
+  <si>
+    <t>Prevalence under 65 Asthma</t>
+  </si>
+  <si>
+    <t>Prevalence under 65 with CKD</t>
+  </si>
+  <si>
+    <t>Prevalence under 65 with Depression</t>
+  </si>
+  <si>
+    <t>Prevalence under 65 with Diabetes</t>
+  </si>
+  <si>
+    <t>Prevalence under 65 with COPS</t>
+  </si>
+  <si>
+    <t>Prevalence under 65 with Heart Failure</t>
+  </si>
+  <si>
+    <t>Prevalence under 65 with Drug Abuse</t>
+  </si>
+  <si>
+    <t>Prevalence under 65 with Hyperlipidemia</t>
+  </si>
+  <si>
+    <t>Prevalence under 65 with Hypertension</t>
+  </si>
+  <si>
+    <t>Prevalence under 65 with Ischemic Heart Disease</t>
+  </si>
+  <si>
+    <t>Prevalence under 65 with Pyschotic Disorders</t>
+  </si>
+  <si>
+    <t>Prevalence over 65 with Alcohol Abuse</t>
+  </si>
+  <si>
+    <t>Prevalence over 65 Arthritis</t>
+  </si>
+  <si>
+    <t>Prevalence over 65 Asthma</t>
+  </si>
+  <si>
+    <t>Prevalence over 65 with CKD</t>
+  </si>
+  <si>
+    <t>Prevalence over 65 with COPS</t>
+  </si>
+  <si>
+    <t>Prevalence over 65 with Depression</t>
+  </si>
+  <si>
+    <t>Prevalence over 65 with Diabetes</t>
+  </si>
+  <si>
+    <t>Prevalence over 65 with Drug Abuse</t>
+  </si>
+  <si>
+    <t>Prevalence over 65 with Heart Failure</t>
+  </si>
+  <si>
+    <t>Prevalence over 65 with Hyperlipidemia</t>
+  </si>
+  <si>
+    <t>Prevalence over 65 with Hypertension</t>
+  </si>
+  <si>
+    <t>Prevalence over 65 with Ischemic Heart Disease</t>
+  </si>
+  <si>
+    <t>Prevalence over 65 with Pyschotic Disorders</t>
+  </si>
+  <si>
+    <t>Ratio Population to Physicians</t>
+  </si>
+  <si>
+    <t>Uninsured Value</t>
+  </si>
+  <si>
+    <t>One Person Household</t>
+  </si>
+  <si>
+    <t>Two Person Household</t>
+  </si>
+  <si>
+    <t>Three Person Household</t>
+  </si>
+  <si>
+    <t>Four Person Household</t>
+  </si>
+  <si>
+    <t>Total Air Quality Summary</t>
+  </si>
+  <si>
+    <t>Average Temperature Feb 2020</t>
+  </si>
+  <si>
+    <t>Average Temperature March 2020</t>
+  </si>
+  <si>
+    <t>Average Temperature April 2020</t>
+  </si>
+  <si>
+    <t>Average Precipitation February 2020</t>
+  </si>
+  <si>
+    <t>Average Precipitation March 2020</t>
+  </si>
+  <si>
+    <t>Average Precipitation April 2020</t>
+  </si>
+  <si>
+    <t>CDC Social Vulnerability Theme 1</t>
+  </si>
+  <si>
+    <t>Percentile Persons Below Poverty Limit</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Percentage Persons Unemployed </t>
+  </si>
+  <si>
+    <t>Percentage Persons with No High School</t>
+  </si>
+  <si>
+    <t>CDC Theme 2</t>
+  </si>
+  <si>
+    <t>CDC Theme 3</t>
+  </si>
+  <si>
+    <t>CDC Theme 4</t>
+  </si>
+  <si>
+    <t>Percentage Housholds More People than Rooms</t>
+  </si>
+  <si>
+    <t>Percentage Houshold with 1 Worker</t>
+  </si>
+  <si>
+    <t>Percentage Houshold with 2 Worker</t>
+  </si>
+  <si>
+    <t>Percentage Houshold with 3 Worker</t>
+  </si>
+  <si>
+    <t>Percentage Unemployed 2018</t>
+  </si>
+  <si>
+    <t>Percentage with Ratio income to poverty at two or greater</t>
+  </si>
+  <si>
+    <t>Commute More than 30 minutes</t>
+  </si>
+  <si>
+    <t>Community Flow to Workplace</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Proportion Male </t>
   </si>
 </sst>
 </file>
@@ -3074,7 +3266,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="12">
+  <cellXfs count="13">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
@@ -3107,6 +3299,7 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -3448,8 +3641,8 @@
   <sheetPr filterMode="1"/>
   <dimension ref="A1:K425"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A155" zoomScale="87" workbookViewId="0">
-      <selection activeCell="J199" sqref="J199"/>
+    <sheetView tabSelected="1" topLeftCell="A123" zoomScale="87" workbookViewId="0">
+      <selection activeCell="F21" sqref="F21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="20.19921875" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
@@ -3569,6 +3762,9 @@
       <c r="B4" s="10" t="s">
         <v>91</v>
       </c>
+      <c r="C4" s="11" t="s">
+        <v>1009</v>
+      </c>
       <c r="D4" s="10" t="s">
         <v>4</v>
       </c>
@@ -3633,6 +3829,9 @@
       <c r="B6" s="10" t="s">
         <v>95</v>
       </c>
+      <c r="C6" s="11" t="s">
+        <v>946</v>
+      </c>
       <c r="D6" s="10" t="s">
         <v>4</v>
       </c>
@@ -4145,6 +4344,9 @@
       <c r="B22" s="10" t="s">
         <v>35</v>
       </c>
+      <c r="C22" s="11" t="s">
+        <v>947</v>
+      </c>
       <c r="D22" s="10" t="s">
         <v>4</v>
       </c>
@@ -4244,6 +4446,9 @@
       <c r="B25" s="10" t="s">
         <v>836</v>
       </c>
+      <c r="C25" s="11" t="s">
+        <v>948</v>
+      </c>
       <c r="D25" s="10" t="s">
         <v>4</v>
       </c>
@@ -4276,6 +4481,9 @@
       <c r="B26" s="10" t="s">
         <v>839</v>
       </c>
+      <c r="C26" s="11" t="s">
+        <v>949</v>
+      </c>
       <c r="D26" s="10" t="s">
         <v>4</v>
       </c>
@@ -4619,6 +4827,9 @@
       <c r="B37" s="10" t="s">
         <v>843</v>
       </c>
+      <c r="C37" s="11" t="s">
+        <v>950</v>
+      </c>
       <c r="D37" s="10" t="s">
         <v>4</v>
       </c>
@@ -4651,6 +4862,9 @@
       <c r="B38" s="10" t="s">
         <v>779</v>
       </c>
+      <c r="C38" s="11" t="s">
+        <v>951</v>
+      </c>
       <c r="D38" s="10" t="s">
         <v>4</v>
       </c>
@@ -4779,6 +4993,9 @@
       <c r="B42" s="10" t="s">
         <v>781</v>
       </c>
+      <c r="C42" s="11" t="s">
+        <v>952</v>
+      </c>
       <c r="D42" s="10" t="s">
         <v>4</v>
       </c>
@@ -5003,6 +5220,9 @@
       <c r="B49" s="10" t="s">
         <v>784</v>
       </c>
+      <c r="C49" s="11" t="s">
+        <v>953</v>
+      </c>
       <c r="D49" s="10" t="s">
         <v>4</v>
       </c>
@@ -5224,6 +5444,9 @@
       <c r="B56" s="10" t="s">
         <v>68</v>
       </c>
+      <c r="C56" s="11" t="s">
+        <v>954</v>
+      </c>
       <c r="D56" s="10" t="s">
         <v>4</v>
       </c>
@@ -5256,6 +5479,9 @@
       <c r="B57" s="10" t="s">
         <v>788</v>
       </c>
+      <c r="C57" s="11" t="s">
+        <v>955</v>
+      </c>
       <c r="D57" s="10" t="s">
         <v>4</v>
       </c>
@@ -5288,6 +5514,9 @@
       <c r="B58" s="10" t="s">
         <v>69</v>
       </c>
+      <c r="C58" s="11" t="s">
+        <v>956</v>
+      </c>
       <c r="D58" s="10" t="s">
         <v>4</v>
       </c>
@@ -5320,6 +5549,9 @@
       <c r="B59" s="10" t="s">
         <v>70</v>
       </c>
+      <c r="C59" s="11" t="s">
+        <v>957</v>
+      </c>
       <c r="D59" s="10" t="s">
         <v>4</v>
       </c>
@@ -5349,6 +5581,9 @@
       <c r="B60" s="10" t="s">
         <v>789</v>
       </c>
+      <c r="C60" s="11" t="s">
+        <v>958</v>
+      </c>
       <c r="D60" s="10" t="s">
         <v>4</v>
       </c>
@@ -5378,6 +5613,9 @@
       <c r="B61" s="10" t="s">
         <v>71</v>
       </c>
+      <c r="C61" s="12" t="s">
+        <v>961</v>
+      </c>
       <c r="D61" s="10" t="s">
         <v>4</v>
       </c>
@@ -5407,6 +5645,9 @@
       <c r="B62" s="10" t="s">
         <v>72</v>
       </c>
+      <c r="C62" s="12" t="s">
+        <v>959</v>
+      </c>
       <c r="D62" s="10" t="s">
         <v>4</v>
       </c>
@@ -5436,6 +5677,9 @@
       <c r="B63" s="10" t="s">
         <v>73</v>
       </c>
+      <c r="C63" s="12" t="s">
+        <v>960</v>
+      </c>
       <c r="D63" s="10" t="s">
         <v>4</v>
       </c>
@@ -5465,6 +5709,9 @@
       <c r="B64" s="10" t="s">
         <v>790</v>
       </c>
+      <c r="C64" s="11" t="s">
+        <v>963</v>
+      </c>
       <c r="D64" s="10" t="s">
         <v>4</v>
       </c>
@@ -5494,6 +5741,9 @@
       <c r="B65" s="10" t="s">
         <v>791</v>
       </c>
+      <c r="C65" s="11" t="s">
+        <v>962</v>
+      </c>
       <c r="D65" s="10" t="s">
         <v>4</v>
       </c>
@@ -5523,6 +5773,9 @@
       <c r="B66" s="10" t="s">
         <v>75</v>
       </c>
+      <c r="C66" s="11" t="s">
+        <v>964</v>
+      </c>
       <c r="D66" s="10" t="s">
         <v>4</v>
       </c>
@@ -5552,6 +5805,9 @@
       <c r="B67" s="10" t="s">
         <v>76</v>
       </c>
+      <c r="C67" s="11" t="s">
+        <v>965</v>
+      </c>
       <c r="D67" s="10" t="s">
         <v>4</v>
       </c>
@@ -5581,6 +5837,9 @@
       <c r="B68" s="10" t="s">
         <v>792</v>
       </c>
+      <c r="C68" s="11" t="s">
+        <v>966</v>
+      </c>
       <c r="D68" s="10" t="s">
         <v>4</v>
       </c>
@@ -5610,6 +5869,9 @@
       <c r="B69" s="10" t="s">
         <v>793</v>
       </c>
+      <c r="C69" s="11" t="s">
+        <v>967</v>
+      </c>
       <c r="D69" s="10" t="s">
         <v>4</v>
       </c>
@@ -5639,6 +5901,9 @@
       <c r="B70" s="10" t="s">
         <v>794</v>
       </c>
+      <c r="C70" s="11" t="s">
+        <v>968</v>
+      </c>
       <c r="D70" s="10" t="s">
         <v>4</v>
       </c>
@@ -5668,6 +5933,9 @@
       <c r="B71" s="10" t="s">
         <v>77</v>
       </c>
+      <c r="C71" s="11" t="s">
+        <v>969</v>
+      </c>
       <c r="D71" s="10" t="s">
         <v>4</v>
       </c>
@@ -5697,6 +5965,9 @@
       <c r="B72" s="10" t="s">
         <v>78</v>
       </c>
+      <c r="C72" s="11" t="s">
+        <v>970</v>
+      </c>
       <c r="D72" s="10" t="s">
         <v>4</v>
       </c>
@@ -5726,6 +5997,9 @@
       <c r="B73" s="10" t="s">
         <v>795</v>
       </c>
+      <c r="C73" s="11" t="s">
+        <v>971</v>
+      </c>
       <c r="D73" s="10" t="s">
         <v>4</v>
       </c>
@@ -5755,6 +6029,9 @@
       <c r="B74" s="10" t="s">
         <v>79</v>
       </c>
+      <c r="C74" s="12" t="s">
+        <v>972</v>
+      </c>
       <c r="D74" s="10" t="s">
         <v>4</v>
       </c>
@@ -5784,6 +6061,9 @@
       <c r="B75" s="10" t="s">
         <v>80</v>
       </c>
+      <c r="C75" s="12" t="s">
+        <v>973</v>
+      </c>
       <c r="D75" s="10" t="s">
         <v>4</v>
       </c>
@@ -5813,6 +6093,9 @@
       <c r="B76" s="10" t="s">
         <v>81</v>
       </c>
+      <c r="C76" s="12" t="s">
+        <v>974</v>
+      </c>
       <c r="D76" s="10" t="s">
         <v>4</v>
       </c>
@@ -5842,6 +6125,9 @@
       <c r="B77" s="10" t="s">
         <v>796</v>
       </c>
+      <c r="C77" s="11" t="s">
+        <v>975</v>
+      </c>
       <c r="D77" s="10" t="s">
         <v>4</v>
       </c>
@@ -5871,6 +6157,9 @@
       <c r="B78" s="10" t="s">
         <v>797</v>
       </c>
+      <c r="C78" s="11" t="s">
+        <v>976</v>
+      </c>
       <c r="D78" s="10" t="s">
         <v>4</v>
       </c>
@@ -5900,6 +6189,9 @@
       <c r="B79" s="10" t="s">
         <v>83</v>
       </c>
+      <c r="C79" s="11" t="s">
+        <v>977</v>
+      </c>
       <c r="D79" s="10" t="s">
         <v>4</v>
       </c>
@@ -5929,6 +6221,9 @@
       <c r="B80" s="10" t="s">
         <v>85</v>
       </c>
+      <c r="C80" s="11" t="s">
+        <v>978</v>
+      </c>
       <c r="D80" s="10" t="s">
         <v>4</v>
       </c>
@@ -5958,6 +6253,9 @@
       <c r="B81" s="10" t="s">
         <v>798</v>
       </c>
+      <c r="C81" s="11" t="s">
+        <v>979</v>
+      </c>
       <c r="D81" s="10" t="s">
         <v>4</v>
       </c>
@@ -5987,6 +6285,9 @@
       <c r="B82" s="10" t="s">
         <v>799</v>
       </c>
+      <c r="C82" s="11" t="s">
+        <v>980</v>
+      </c>
       <c r="D82" s="10" t="s">
         <v>4</v>
       </c>
@@ -6112,6 +6413,9 @@
       <c r="B86" s="10" t="s">
         <v>48</v>
       </c>
+      <c r="C86" s="11" t="s">
+        <v>981</v>
+      </c>
       <c r="D86" s="10" t="s">
         <v>4</v>
       </c>
@@ -6208,6 +6512,9 @@
       <c r="B89" s="10" t="s">
         <v>291</v>
       </c>
+      <c r="C89" s="11" t="s">
+        <v>982</v>
+      </c>
       <c r="D89" s="10" t="s">
         <v>4</v>
       </c>
@@ -6272,6 +6579,9 @@
       <c r="B91" s="10" t="s">
         <v>120</v>
       </c>
+      <c r="C91" s="11" t="s">
+        <v>983</v>
+      </c>
       <c r="D91" s="10" t="s">
         <v>4</v>
       </c>
@@ -6304,6 +6614,9 @@
       <c r="B92" s="10" t="s">
         <v>123</v>
       </c>
+      <c r="C92" s="11" t="s">
+        <v>984</v>
+      </c>
       <c r="D92" s="10" t="s">
         <v>4</v>
       </c>
@@ -6333,6 +6646,9 @@
       <c r="B93" s="10" t="s">
         <v>125</v>
       </c>
+      <c r="C93" s="11" t="s">
+        <v>985</v>
+      </c>
       <c r="D93" s="10" t="s">
         <v>4</v>
       </c>
@@ -6362,6 +6678,9 @@
       <c r="B94" s="10" t="s">
         <v>127</v>
       </c>
+      <c r="C94" s="11" t="s">
+        <v>986</v>
+      </c>
       <c r="D94" s="10" t="s">
         <v>4</v>
       </c>
@@ -6626,6 +6945,9 @@
       <c r="B103" s="10" t="s">
         <v>33</v>
       </c>
+      <c r="C103" s="11" t="s">
+        <v>987</v>
+      </c>
       <c r="D103" s="10" t="s">
         <v>4</v>
       </c>
@@ -6800,6 +7122,9 @@
       <c r="B109" s="10" t="s">
         <v>146</v>
       </c>
+      <c r="C109" s="11" t="s">
+        <v>988</v>
+      </c>
       <c r="D109" s="10" t="s">
         <v>4</v>
       </c>
@@ -6832,6 +7157,9 @@
       <c r="B110" s="10" t="s">
         <v>148</v>
       </c>
+      <c r="C110" s="11" t="s">
+        <v>989</v>
+      </c>
       <c r="D110" s="10" t="s">
         <v>4</v>
       </c>
@@ -6864,6 +7192,9 @@
       <c r="B111" s="10" t="s">
         <v>150</v>
       </c>
+      <c r="C111" s="11" t="s">
+        <v>990</v>
+      </c>
       <c r="D111" s="10" t="s">
         <v>4</v>
       </c>
@@ -7073,6 +7404,9 @@
       <c r="B118" s="10" t="s">
         <v>152</v>
       </c>
+      <c r="C118" s="11" t="s">
+        <v>991</v>
+      </c>
       <c r="D118" s="10" t="s">
         <v>4</v>
       </c>
@@ -7102,6 +7436,9 @@
       <c r="B119" s="10" t="s">
         <v>154</v>
       </c>
+      <c r="C119" s="11" t="s">
+        <v>992</v>
+      </c>
       <c r="D119" s="10" t="s">
         <v>4</v>
       </c>
@@ -7131,6 +7468,9 @@
       <c r="B120" s="10" t="s">
         <v>156</v>
       </c>
+      <c r="C120" s="11" t="s">
+        <v>993</v>
+      </c>
       <c r="D120" s="10" t="s">
         <v>4</v>
       </c>
@@ -7320,6 +7660,9 @@
       <c r="B126" s="10" t="s">
         <v>87</v>
       </c>
+      <c r="C126" s="11" t="s">
+        <v>994</v>
+      </c>
       <c r="D126" s="10" t="s">
         <v>4</v>
       </c>
@@ -7349,6 +7692,9 @@
       <c r="B127" s="10" t="s">
         <v>196</v>
       </c>
+      <c r="C127" s="11" t="s">
+        <v>995</v>
+      </c>
       <c r="F127" s="10" t="s">
         <v>811</v>
       </c>
@@ -7372,6 +7718,9 @@
       <c r="B128" s="10" t="s">
         <v>198</v>
       </c>
+      <c r="C128" s="11" t="s">
+        <v>996</v>
+      </c>
       <c r="F128" s="10" t="s">
         <v>811</v>
       </c>
@@ -7418,6 +7767,9 @@
       <c r="B130" s="10" t="s">
         <v>202</v>
       </c>
+      <c r="C130" s="11" t="s">
+        <v>997</v>
+      </c>
       <c r="F130" s="10" t="s">
         <v>811</v>
       </c>
@@ -7444,6 +7796,9 @@
       <c r="B131" s="10" t="s">
         <v>88</v>
       </c>
+      <c r="C131" s="11" t="s">
+        <v>998</v>
+      </c>
       <c r="D131" s="10" t="s">
         <v>4</v>
       </c>
@@ -7568,6 +7923,9 @@
       <c r="B136" s="10" t="s">
         <v>89</v>
       </c>
+      <c r="C136" s="11" t="s">
+        <v>999</v>
+      </c>
       <c r="D136" s="10" t="s">
         <v>4</v>
       </c>
@@ -7643,6 +8001,9 @@
       <c r="B139" s="10" t="s">
         <v>90</v>
       </c>
+      <c r="C139" s="11" t="s">
+        <v>1000</v>
+      </c>
       <c r="D139" s="10" t="s">
         <v>4</v>
       </c>
@@ -7715,6 +8076,9 @@
       <c r="B142" s="10" t="s">
         <v>219</v>
       </c>
+      <c r="C142" s="11" t="s">
+        <v>1001</v>
+      </c>
       <c r="F142" s="10" t="s">
         <v>811</v>
       </c>
@@ -7825,7 +8189,9 @@
       <c r="B146" s="4" t="s">
         <v>114</v>
       </c>
-      <c r="C146" s="4"/>
+      <c r="C146" s="4" t="s">
+        <v>1002</v>
+      </c>
       <c r="D146" s="4" t="s">
         <v>4</v>
       </c>
@@ -7858,7 +8224,9 @@
       <c r="B147" s="4" t="s">
         <v>116</v>
       </c>
-      <c r="C147" s="4"/>
+      <c r="C147" s="4" t="s">
+        <v>1003</v>
+      </c>
       <c r="D147" s="4" t="s">
         <v>4</v>
       </c>
@@ -7888,7 +8256,9 @@
       <c r="B148" s="4" t="s">
         <v>118</v>
       </c>
-      <c r="C148" s="4"/>
+      <c r="C148" s="4" t="s">
+        <v>1004</v>
+      </c>
       <c r="D148" s="4" t="s">
         <v>4</v>
       </c>
@@ -7918,7 +8288,9 @@
       <c r="B149" s="4" t="s">
         <v>132</v>
       </c>
-      <c r="C149" s="4"/>
+      <c r="C149" s="4" t="s">
+        <v>1005</v>
+      </c>
       <c r="D149" s="4" t="s">
         <v>4</v>
       </c>
@@ -8018,7 +8390,9 @@
       <c r="B152" s="4" t="s">
         <v>139</v>
       </c>
-      <c r="C152" s="4"/>
+      <c r="C152" s="4" t="s">
+        <v>1006</v>
+      </c>
       <c r="D152" s="4" t="s">
         <v>4</v>
       </c>
@@ -8083,7 +8457,9 @@
       <c r="B154" s="5" t="s">
         <v>53</v>
       </c>
-      <c r="C154" s="5"/>
+      <c r="C154" s="5" t="s">
+        <v>1007</v>
+      </c>
       <c r="D154" s="4" t="s">
         <v>4</v>
       </c>
@@ -8177,7 +8553,9 @@
       <c r="B157" s="4" t="s">
         <v>144</v>
       </c>
-      <c r="C157" s="4"/>
+      <c r="C157" s="4" t="s">
+        <v>1008</v>
+      </c>
       <c r="D157" s="4" t="s">
         <v>4</v>
       </c>

</xml_diff>

<commit_message>
testing joint shift with new models.
</commit_message>
<xml_diff>
--- a/data/processed/Data_Dictionary.xlsx
+++ b/data/processed/Data_Dictionary.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="10215"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="10410"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/davidmccoy/COVIDxrisk/data/processed/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8357905C-B83B-254C-997A-DE4EFC1DD806}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DBC24BD0-ABFD-9E47-AEFF-EBB3FAC95B18}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="30440" yWindow="500" windowWidth="48940" windowHeight="25540" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -3632,8 +3632,8 @@
   <sheetPr filterMode="1"/>
   <dimension ref="A1:K425"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A137" zoomScale="87" workbookViewId="0">
-      <selection activeCell="H144" sqref="H144"/>
+    <sheetView tabSelected="1" topLeftCell="A304" zoomScale="87" workbookViewId="0">
+      <selection activeCell="F354" sqref="F354"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="20.19921875" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
@@ -12357,7 +12357,7 @@
         <v>764</v>
       </c>
       <c r="F349" s="9" t="s">
-        <v>811</v>
+        <v>831</v>
       </c>
       <c r="G349" s="9" t="s">
         <v>850</v>
@@ -12374,7 +12374,7 @@
         <v>765</v>
       </c>
       <c r="F350" s="9" t="s">
-        <v>811</v>
+        <v>831</v>
       </c>
       <c r="G350" s="9" t="s">
         <v>850</v>
@@ -12391,7 +12391,7 @@
         <v>766</v>
       </c>
       <c r="F351" s="9" t="s">
-        <v>811</v>
+        <v>831</v>
       </c>
       <c r="G351" s="9" t="s">
         <v>850</v>
@@ -12408,7 +12408,7 @@
         <v>767</v>
       </c>
       <c r="F352" s="9" t="s">
-        <v>811</v>
+        <v>831</v>
       </c>
       <c r="G352" s="9" t="s">
         <v>850</v>
@@ -12425,7 +12425,7 @@
         <v>768</v>
       </c>
       <c r="F353" s="9" t="s">
-        <v>811</v>
+        <v>831</v>
       </c>
       <c r="G353" s="9" t="s">
         <v>850</v>

</xml_diff>

<commit_message>
Updates to preprocessing to create new data.
</commit_message>
<xml_diff>
--- a/data/processed/Data_Dictionary.xlsx
+++ b/data/processed/Data_Dictionary.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="10410"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="10611"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/davidmccoy/COVIDxrisk/data/processed/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DBC24BD0-ABFD-9E47-AEFF-EBB3FAC95B18}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A5494CF2-1F3C-5F49-AC43-F2E6083A95A3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="30440" yWindow="500" windowWidth="48940" windowHeight="25540" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-51200" yWindow="0" windowWidth="51200" windowHeight="28800" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Table 1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3196" uniqueCount="1010">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3864" uniqueCount="1305">
   <si>
     <t>Col Num</t>
   </si>
@@ -3189,12 +3189,897 @@
   <si>
     <t xml:space="preserve">Proportion Male </t>
   </si>
+  <si>
+    <t>blackwhitegap</t>
+  </si>
+  <si>
+    <t>hispwhitegap</t>
+  </si>
+  <si>
+    <t>asianwhitegap</t>
+  </si>
+  <si>
+    <t>AreaWater</t>
+  </si>
+  <si>
+    <t>Poor.or.fair.health.raw.value</t>
+  </si>
+  <si>
+    <t>Low.birthweight.raw.value</t>
+  </si>
+  <si>
+    <t>Physical.inactivity.raw.value</t>
+  </si>
+  <si>
+    <t>Alcohol.impaired.driving.deaths.raw.value</t>
+  </si>
+  <si>
+    <t>Teen.births.raw.value</t>
+  </si>
+  <si>
+    <t>Ratio.of.population.to.primary.care.physicians.</t>
+  </si>
+  <si>
+    <t>Dentists.raw.value</t>
+  </si>
+  <si>
+    <t>Mental.health.providers.raw.value</t>
+  </si>
+  <si>
+    <t>Mammography.screening.raw.value</t>
+  </si>
+  <si>
+    <t>Children.in.poverty.raw.value</t>
+  </si>
+  <si>
+    <t>Children.in.single.parent.households.raw.value</t>
+  </si>
+  <si>
+    <t>Violent.crime.raw.value</t>
+  </si>
+  <si>
+    <t>Injury.deaths.raw.value</t>
+  </si>
+  <si>
+    <t>Severe.housing.problems.raw.value</t>
+  </si>
+  <si>
+    <t>Long.commute...driving.alone.raw.value</t>
+  </si>
+  <si>
+    <t>Premature.age.adjusted.mortality.raw.value</t>
+  </si>
+  <si>
+    <t>Child.mortality.raw.value</t>
+  </si>
+  <si>
+    <t>Infant.mortality.raw.value</t>
+  </si>
+  <si>
+    <t>Diabetes.prevalence.raw.value</t>
+  </si>
+  <si>
+    <t>Limited.access.to.healthy.foods.raw.value</t>
+  </si>
+  <si>
+    <t>Drug.overdose.deaths.raw.value</t>
+  </si>
+  <si>
+    <t>Motor.vehicle.crash.deaths.raw.value</t>
+  </si>
+  <si>
+    <t>Uninsured.children.raw.value</t>
+  </si>
+  <si>
+    <t>Other.primary.care.providers.raw.value</t>
+  </si>
+  <si>
+    <t>Disconnected.youth.raw.value</t>
+  </si>
+  <si>
+    <t>Reading.scores.raw.value</t>
+  </si>
+  <si>
+    <t>Children.eligible.for.free.or.reduced.price.lunch.raw.value</t>
+  </si>
+  <si>
+    <t>Residential.segregation...non.White.White.raw.value</t>
+  </si>
+  <si>
+    <t>Homicides.raw.value</t>
+  </si>
+  <si>
+    <t>Suicides.raw.value</t>
+  </si>
+  <si>
+    <t>Firearm.fatalities.raw.value</t>
+  </si>
+  <si>
+    <t>Traffic.volume.raw.value</t>
+  </si>
+  <si>
+    <t>Homeownership.raw.value</t>
+  </si>
+  <si>
+    <t>Severe.housing.cost.burden.raw.value</t>
+  </si>
+  <si>
+    <t>X..Native.Hawaiian.Other.Pacific.Islander.raw.value</t>
+  </si>
+  <si>
+    <t>X..Non.Hispanic.White.raw.value</t>
+  </si>
+  <si>
+    <t>X..Females.raw.value</t>
+  </si>
+  <si>
+    <t>X..Rural.raw.value</t>
+  </si>
+  <si>
+    <t>prev_2017_all_ages_Autism Spectrum Disorders</t>
+  </si>
+  <si>
+    <t>prev_2017_all_ages_HIV/AIDS</t>
+  </si>
+  <si>
+    <t>prev_2017_under_65_Alzheimer's Disease/Dementia</t>
+  </si>
+  <si>
+    <t>prev_2017_under_65_Atrial Fibrillation</t>
+  </si>
+  <si>
+    <t>prev_2017_under_65_Autism Spectrum Disorders</t>
+  </si>
+  <si>
+    <t>prev_2017_under_65_Cancer</t>
+  </si>
+  <si>
+    <t>prev_2017_under_65_HIV/AIDS</t>
+  </si>
+  <si>
+    <t>prev_2017_under_65_Hepatitis                                 (Chronic Viral B &amp; C)</t>
+  </si>
+  <si>
+    <t>prev_2017_under_65_Osteoporosis</t>
+  </si>
+  <si>
+    <t>prev_2017_under_65_Stroke</t>
+  </si>
+  <si>
+    <t>prev_2017_over_65_Alzheimer's Disease/Dementia</t>
+  </si>
+  <si>
+    <t>prev_2017_over_65_Atrial Fibrillation</t>
+  </si>
+  <si>
+    <t>prev_2017_over_65_Autism Spectrum Disorders</t>
+  </si>
+  <si>
+    <t>prev_2017_over_65_Cancer</t>
+  </si>
+  <si>
+    <t>prev_2017_over_65_HIV/AIDS</t>
+  </si>
+  <si>
+    <t>prev_2017_over_65_Hepatitis                                 (Chronic Viral B &amp; C)</t>
+  </si>
+  <si>
+    <t>prev_2017_over_65_Osteoporosis</t>
+  </si>
+  <si>
+    <t>prev_2017_over_65_Stroke</t>
+  </si>
+  <si>
+    <t>M_HH</t>
+  </si>
+  <si>
+    <t>M_AGE65</t>
+  </si>
+  <si>
+    <t>M_SNGPNT</t>
+  </si>
+  <si>
+    <t>E_MINRTY</t>
+  </si>
+  <si>
+    <t>M_MINRTY</t>
+  </si>
+  <si>
+    <t>E_LIMENG</t>
+  </si>
+  <si>
+    <t>M_LIMENG</t>
+  </si>
+  <si>
+    <t>E_MUNIT</t>
+  </si>
+  <si>
+    <t>M_MUNIT</t>
+  </si>
+  <si>
+    <t>E_MOBILE</t>
+  </si>
+  <si>
+    <t>M_MOBILE</t>
+  </si>
+  <si>
+    <t>E_CROWD</t>
+  </si>
+  <si>
+    <t>M_CROWD</t>
+  </si>
+  <si>
+    <t>E_NOVEH</t>
+  </si>
+  <si>
+    <t>M_NOVEH</t>
+  </si>
+  <si>
+    <t>E_GROUPQ</t>
+  </si>
+  <si>
+    <t>M_GROUPQ</t>
+  </si>
+  <si>
+    <t>EP_PCI</t>
+  </si>
+  <si>
+    <t>MP_PCI</t>
+  </si>
+  <si>
+    <t>EP_NOHSDP</t>
+  </si>
+  <si>
+    <t>MP_NOHSDP</t>
+  </si>
+  <si>
+    <t>EP_AGE65</t>
+  </si>
+  <si>
+    <t>MP_AGE65</t>
+  </si>
+  <si>
+    <t>EP_AGE17</t>
+  </si>
+  <si>
+    <t>MP_AGE17</t>
+  </si>
+  <si>
+    <t>MP_DISABL</t>
+  </si>
+  <si>
+    <t>EP_SNGPNT</t>
+  </si>
+  <si>
+    <t>MP_SNGPNT</t>
+  </si>
+  <si>
+    <t>EP_MINRTY</t>
+  </si>
+  <si>
+    <t>MP_MINRTY</t>
+  </si>
+  <si>
+    <t>EP_LIMENG</t>
+  </si>
+  <si>
+    <t>MP_LIMENG</t>
+  </si>
+  <si>
+    <t>EP_MUNIT</t>
+  </si>
+  <si>
+    <t>MP_MUNIT</t>
+  </si>
+  <si>
+    <t>EP_MOBILE</t>
+  </si>
+  <si>
+    <t>MP_MOBILE</t>
+  </si>
+  <si>
+    <t>EP_CROWD</t>
+  </si>
+  <si>
+    <t>MP_CROWD</t>
+  </si>
+  <si>
+    <t>EP_NOVEH</t>
+  </si>
+  <si>
+    <t>MP_NOVEH</t>
+  </si>
+  <si>
+    <t>EP_GROUPQ</t>
+  </si>
+  <si>
+    <t>MP_GROUPQ</t>
+  </si>
+  <si>
+    <t>F_NOHSDP</t>
+  </si>
+  <si>
+    <t>F_AGE65</t>
+  </si>
+  <si>
+    <t>F_AGE17</t>
+  </si>
+  <si>
+    <t>F_DISABL</t>
+  </si>
+  <si>
+    <t>F_SNGPNT</t>
+  </si>
+  <si>
+    <t>F_THEME2</t>
+  </si>
+  <si>
+    <t>F_MINRTY</t>
+  </si>
+  <si>
+    <t>F_LIMENG</t>
+  </si>
+  <si>
+    <t>F_THEME3</t>
+  </si>
+  <si>
+    <t>F_MUNIT</t>
+  </si>
+  <si>
+    <t>F_MOBILE</t>
+  </si>
+  <si>
+    <t>F_CROWD</t>
+  </si>
+  <si>
+    <t>F_NOVEH</t>
+  </si>
+  <si>
+    <t>F_GROUPQ</t>
+  </si>
+  <si>
+    <t>F_THEME4</t>
+  </si>
+  <si>
+    <t>F_TOTAL</t>
+  </si>
+  <si>
+    <t>E_UNINSUR</t>
+  </si>
+  <si>
+    <t>EP_UNINSUR</t>
+  </si>
+  <si>
+    <t>MP_UNINSUR</t>
+  </si>
+  <si>
+    <t>E_DAYPOP</t>
+  </si>
+  <si>
+    <t>median_age_2018</t>
+  </si>
+  <si>
+    <t>pct_1.person_household_2018</t>
+  </si>
+  <si>
+    <t>pct_2.person_household_2018</t>
+  </si>
+  <si>
+    <t>pct_3.person_household_2018</t>
+  </si>
+  <si>
+    <t>pct_4.or.more.person_household_2018</t>
+  </si>
+  <si>
+    <t>arsenic_avgs</t>
+  </si>
+  <si>
+    <t>ALACHLOR</t>
+  </si>
+  <si>
+    <t>CHLORIMURON</t>
+  </si>
+  <si>
+    <t>CLOMAZONE</t>
+  </si>
+  <si>
+    <t>CYPROCONAZOLE</t>
+  </si>
+  <si>
+    <t>FAMOXADONE</t>
+  </si>
+  <si>
+    <t>FLUAZIFOP</t>
+  </si>
+  <si>
+    <t>LINURON</t>
+  </si>
+  <si>
+    <t>METHOMYL</t>
+  </si>
+  <si>
+    <t>MYCLOBUTANIL</t>
+  </si>
+  <si>
+    <t>OXAMYL</t>
+  </si>
+  <si>
+    <t>PHOSPHORIC ACID</t>
+  </si>
+  <si>
+    <t>PROSULFURON</t>
+  </si>
+  <si>
+    <t>QUIZALOFOP</t>
+  </si>
+  <si>
+    <t>SPINOSYN</t>
+  </si>
+  <si>
+    <t>TEFLUTHRIN</t>
+  </si>
+  <si>
+    <t>TERBUFOS</t>
+  </si>
+  <si>
+    <t>ACEPHATE</t>
+  </si>
+  <si>
+    <t>ACETAMIPRID</t>
+  </si>
+  <si>
+    <t>BACILLUS THURINGIENSIS</t>
+  </si>
+  <si>
+    <t>BOSCALID</t>
+  </si>
+  <si>
+    <t>COPPER</t>
+  </si>
+  <si>
+    <t>COPPER SULFATE</t>
+  </si>
+  <si>
+    <t>FLUOXASTROBIN</t>
+  </si>
+  <si>
+    <t>MANDIPROPAMID</t>
+  </si>
+  <si>
+    <t>PETROLEUM OIL</t>
+  </si>
+  <si>
+    <t>PHOSMET</t>
+  </si>
+  <si>
+    <t>PYRAFLUFEN ETHYL</t>
+  </si>
+  <si>
+    <t>TOPRAMEZONE</t>
+  </si>
+  <si>
+    <t>BENZOVINDIFLUPYR</t>
+  </si>
+  <si>
+    <t>FENTIN</t>
+  </si>
+  <si>
+    <t>FLUBENDIAMIDE</t>
+  </si>
+  <si>
+    <t>FLUOPYRAM</t>
+  </si>
+  <si>
+    <t>GIBBERELLIC ACID</t>
+  </si>
+  <si>
+    <t>PICOXYSTROBIN</t>
+  </si>
+  <si>
+    <t>SEDAXANE</t>
+  </si>
+  <si>
+    <t>TETRACONAZOLE</t>
+  </si>
+  <si>
+    <t>THIRAM</t>
+  </si>
+  <si>
+    <t>PINOXADEN</t>
+  </si>
+  <si>
+    <t>PYROXSULAM</t>
+  </si>
+  <si>
+    <t>Chetty opportunity score, Black-white gap</t>
+  </si>
+  <si>
+    <t>Chetty opportunity score, Hispanic-white gap</t>
+  </si>
+  <si>
+    <t>Chetty opportunity score, Asian-white gap</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Water Area </t>
+  </si>
+  <si>
+    <t>Poor or Fair Health</t>
+  </si>
+  <si>
+    <t>Low Birthweight</t>
+  </si>
+  <si>
+    <t>Physical Activity</t>
+  </si>
+  <si>
+    <t>Alcohol Impaired Driving Deaths</t>
+  </si>
+  <si>
+    <t>Teen Births</t>
+  </si>
+  <si>
+    <t>Ratio Primary Care Physicians</t>
+  </si>
+  <si>
+    <t>Dentists</t>
+  </si>
+  <si>
+    <t>Mental Health Providers</t>
+  </si>
+  <si>
+    <t>Mammography Screening</t>
+  </si>
+  <si>
+    <t>Child Poverty</t>
+  </si>
+  <si>
+    <t>Children in Single Parent Households</t>
+  </si>
+  <si>
+    <t>Violent Crimes</t>
+  </si>
+  <si>
+    <t>Injury Deaths</t>
+  </si>
+  <si>
+    <t>Severe Housing Problems</t>
+  </si>
+  <si>
+    <t>Long Communting Alone</t>
+  </si>
+  <si>
+    <t>Premature Mortalities</t>
+  </si>
+  <si>
+    <t>Child Mortality</t>
+  </si>
+  <si>
+    <t>Infant Mortality</t>
+  </si>
+  <si>
+    <t>Diabetes</t>
+  </si>
+  <si>
+    <t>Limited Acess to Healthy Foods</t>
+  </si>
+  <si>
+    <t>Drug Overdoses</t>
+  </si>
+  <si>
+    <t>Motor Vehicle Crashes</t>
+  </si>
+  <si>
+    <t>Uninsured Children</t>
+  </si>
+  <si>
+    <t>Other Primary Care Physicians</t>
+  </si>
+  <si>
+    <t>Disconnected Youth</t>
+  </si>
+  <si>
+    <t>Reading Scores</t>
+  </si>
+  <si>
+    <t>Children Eligible for Reduced Lunch Prices</t>
+  </si>
+  <si>
+    <t>Non-White White Segregation</t>
+  </si>
+  <si>
+    <t>Homicides</t>
+  </si>
+  <si>
+    <t>Suicides</t>
+  </si>
+  <si>
+    <t>Firearm Fatalities</t>
+  </si>
+  <si>
+    <t>Traffic Volume</t>
+  </si>
+  <si>
+    <t>Homeownership</t>
+  </si>
+  <si>
+    <t>Severe Housing Cost Burden</t>
+  </si>
+  <si>
+    <t>Native Hawaiian Other Pacific Islander</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Non Hispanic White </t>
+  </si>
+  <si>
+    <t>Females</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Rural </t>
+  </si>
+  <si>
+    <t>Prevalence ASD</t>
+  </si>
+  <si>
+    <t>Prevalence HIV/AIDS</t>
+  </si>
+  <si>
+    <t>Prevalence ASD under 65</t>
+  </si>
+  <si>
+    <t>Prevalence Cancer under 65</t>
+  </si>
+  <si>
+    <t>Prevalence HIV/AIDS under 65</t>
+  </si>
+  <si>
+    <t>Prevalence Alzheimer's under 65</t>
+  </si>
+  <si>
+    <t>Prevalence Hepatitis under 65</t>
+  </si>
+  <si>
+    <t>Prevalence Osteoporosis under 65</t>
+  </si>
+  <si>
+    <t>Prevalence Stroke under 65</t>
+  </si>
+  <si>
+    <t>Prevalence Alzheimer's over 65</t>
+  </si>
+  <si>
+    <t>Prevalence Atrial Fibrillation over 65</t>
+  </si>
+  <si>
+    <t>Prevalence Atrial Fibrillation under 65</t>
+  </si>
+  <si>
+    <t>Prevalence ASD over 65</t>
+  </si>
+  <si>
+    <t>Prevalence Cancer over 65</t>
+  </si>
+  <si>
+    <t>Prevalence HIV/AIDS over 65</t>
+  </si>
+  <si>
+    <t>Prevalence Hepatitis over 65</t>
+  </si>
+  <si>
+    <t>Prevalence Osteoporosis over 65</t>
+  </si>
+  <si>
+    <t>Prevalence Stroke over 65</t>
+  </si>
+  <si>
+    <t>Households estimate MOE</t>
+  </si>
+  <si>
+    <t>Persons aged 65 and older estimate MOE</t>
+  </si>
+  <si>
+    <t>Single parent household with children under 18 estimate MOE</t>
+  </si>
+  <si>
+    <t>Minority (all persons except white, non - Hispanic) estimate</t>
+  </si>
+  <si>
+    <t>Minority (all persons except white, non - Hispanic) estimate MOE</t>
+  </si>
+  <si>
+    <t>Persons (age 5+) who speak English "less than well" estimate</t>
+  </si>
+  <si>
+    <t>Persons (age 5+) who speak English "less than well" estimate MOE</t>
+  </si>
+  <si>
+    <t>Housing in structures with 10 or more units estimate,</t>
+  </si>
+  <si>
+    <t>Housing in structures with 10 or more units estimate MOE</t>
+  </si>
+  <si>
+    <t>Mobile homes estimate</t>
+  </si>
+  <si>
+    <t>Mobile homes estimate MOE</t>
+  </si>
+  <si>
+    <t>At household level (occupied housing units), more people than rooms estimate</t>
+  </si>
+  <si>
+    <t>At household level (occupied housing units), more people than rooms estimate MOE</t>
+  </si>
+  <si>
+    <t>Households with no vehicle available estimate</t>
+  </si>
+  <si>
+    <t>Households with no vehicle available estimate MOE</t>
+  </si>
+  <si>
+    <t>Persons in group quarters estimate</t>
+  </si>
+  <si>
+    <t>Persons in group quarters estimate MOE</t>
+  </si>
+  <si>
+    <t>Per capita income estimate</t>
+  </si>
+  <si>
+    <t>Per capita income estimate MOE</t>
+  </si>
+  <si>
+    <t>Percentage of persons with no high school diploma</t>
+  </si>
+  <si>
+    <t>Percentage of persons with no high school diploma MOE</t>
+  </si>
+  <si>
+    <t>Percentage of persons aged 65 and older estimate</t>
+  </si>
+  <si>
+    <t>Percentage of persons aged 65 and older estimate MOE</t>
+  </si>
+  <si>
+    <t>Percentage of persons aged 17 and younger estimate</t>
+  </si>
+  <si>
+    <t>Percentage of persons aged 17 and younger estimate MOE</t>
+  </si>
+  <si>
+    <t>Percentage of civilian noninstitutiona lized population with a disability estimate MOE</t>
+  </si>
+  <si>
+    <t>Percentage of single parent households with children under 18 estimate,</t>
+  </si>
+  <si>
+    <t>Percentage of single parent households with children under 18 estimate MOE</t>
+  </si>
+  <si>
+    <t>Percentage minority (all persons except white, nonHispanic) estimate,</t>
+  </si>
+  <si>
+    <t>Percentage minority (all persons except white, nonHispanic) estimate MOE</t>
+  </si>
+  <si>
+    <t>Percentage of persons (age 5+) who speak English "less than well" estimate</t>
+  </si>
+  <si>
+    <t>Percentage of persons (age 5+) who speak English "less than well" estimate MOE</t>
+  </si>
+  <si>
+    <t>Percentage of housing in structures with 10 or more units estimate</t>
+  </si>
+  <si>
+    <t>Percentage of housing in structures with 10 or more units estimate MOE</t>
+  </si>
+  <si>
+    <t>Percentage of mobile homes estimate</t>
+  </si>
+  <si>
+    <t>Percentage of mobile homes estimate MOE</t>
+  </si>
+  <si>
+    <t>Percentage of occupied housing units with more people than rooms estimate</t>
+  </si>
+  <si>
+    <t>Percentage of occupied housing units with more people than rooms estimate MOE</t>
+  </si>
+  <si>
+    <t>Percentage of households with no vehicle available estimate</t>
+  </si>
+  <si>
+    <t>Percentage of households with no vehicle available estimate MOE</t>
+  </si>
+  <si>
+    <t>Percentage of persons in group quarters estimate</t>
+  </si>
+  <si>
+    <t>Percentage of persons in group quarters estimate MOE</t>
+  </si>
+  <si>
+    <t>Flag - the percentage of persons with no high school diploma is in the 90th percentile</t>
+  </si>
+  <si>
+    <t>Flag - the percentage of persons aged 65 and older is in the 90th percentile</t>
+  </si>
+  <si>
+    <t>Flag - the percentage of persons aged 17 and younger is in the 90th percentile (</t>
+  </si>
+  <si>
+    <t>Flag - the percentage of persons with a disability is in the 90th percentile</t>
+  </si>
+  <si>
+    <t>Flag - the percentage of single parent households is in the 90th percentile</t>
+  </si>
+  <si>
+    <t>Sum of flags for Household Composition theme</t>
+  </si>
+  <si>
+    <t>Flag - the percentage of minority is in the 90th percentile</t>
+  </si>
+  <si>
+    <t>Flag - the percentage those with limited English is in the 90th percentile</t>
+  </si>
+  <si>
+    <t>Sum of flags for Minority Status/Languag e theme</t>
+  </si>
+  <si>
+    <t>Flag - the percentage of households in multi -unit housing is in the 90th percentile</t>
+  </si>
+  <si>
+    <t>Flag - the percentage of mobile homes is in the 90th percentile</t>
+  </si>
+  <si>
+    <t>Flag - the percentage of crowded households is in the 90th percentile</t>
+  </si>
+  <si>
+    <t>Flag - the percentage of households with no vehicles is in the 90th percentile</t>
+  </si>
+  <si>
+    <t>Flag - the percentage of persons in institutionalize d group quarters is in the 90th percentile</t>
+  </si>
+  <si>
+    <t>Sum of flags for Housing Type / Transportation theme</t>
+  </si>
+  <si>
+    <t>Sum of flags for the four themes</t>
+  </si>
+  <si>
+    <t>Uninsured in the total civilian noninstitutiona lized population estimate</t>
+  </si>
+  <si>
+    <t>Percentage uninsured in the total civilian noninstitutiona lized population estimate</t>
+  </si>
+  <si>
+    <t>Percentage uninsured in the total civilian noninstitutiona lized population estimate MOE</t>
+  </si>
+  <si>
+    <t>Estimated daytime population</t>
+  </si>
+  <si>
+    <t>Median age as of 2018</t>
+  </si>
+  <si>
+    <t>Percent 1 person households</t>
+  </si>
+  <si>
+    <t>Percent 2 person households</t>
+  </si>
+  <si>
+    <t>Percent 3 person households</t>
+  </si>
+  <si>
+    <t>Percent 4 person households</t>
+  </si>
+  <si>
+    <t>Average Arsenic Values</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="5" x14ac:knownFonts="1">
+  <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="10"/>
       <color rgb="FF000000"/>
@@ -3222,6 +4107,12 @@
       <u/>
       <sz val="10"/>
       <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
       <family val="2"/>
     </font>
   </fonts>
@@ -3260,7 +4151,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="12">
+  <cellXfs count="14">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
@@ -3291,6 +4182,10 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -3630,10 +4525,10 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <sheetPr filterMode="1"/>
-  <dimension ref="A1:K425"/>
+  <dimension ref="A1:K592"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A304" zoomScale="87" workbookViewId="0">
-      <selection activeCell="F354" sqref="F354"/>
+    <sheetView tabSelected="1" topLeftCell="A389" zoomScale="87" workbookViewId="0">
+      <selection activeCell="H446" sqref="H446"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="20.19921875" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
@@ -13654,7 +14549,2345 @@
       <c r="G425" s="9" t="s">
         <v>810</v>
       </c>
-      <c r="J425" s="9" t="s">
+      <c r="J425" s="10" t="s">
+        <v>161</v>
+      </c>
+    </row>
+    <row r="426" spans="2:10" ht="16" x14ac:dyDescent="0.2">
+      <c r="B426" s="9" t="s">
+        <v>1010</v>
+      </c>
+      <c r="C426" s="12" t="s">
+        <v>1177</v>
+      </c>
+      <c r="F426" s="9" t="s">
+        <v>856</v>
+      </c>
+      <c r="J426" s="10" t="s">
+        <v>161</v>
+      </c>
+    </row>
+    <row r="427" spans="2:10" ht="16" x14ac:dyDescent="0.2">
+      <c r="B427" s="9" t="s">
+        <v>1011</v>
+      </c>
+      <c r="C427" s="12" t="s">
+        <v>1178</v>
+      </c>
+      <c r="F427" s="9" t="s">
+        <v>856</v>
+      </c>
+      <c r="J427" s="10" t="s">
+        <v>161</v>
+      </c>
+    </row>
+    <row r="428" spans="2:10" ht="16" x14ac:dyDescent="0.2">
+      <c r="B428" s="9" t="s">
+        <v>1012</v>
+      </c>
+      <c r="C428" s="12" t="s">
+        <v>1179</v>
+      </c>
+      <c r="F428" s="9" t="s">
+        <v>856</v>
+      </c>
+      <c r="J428" s="10" t="s">
+        <v>161</v>
+      </c>
+    </row>
+    <row r="429" spans="2:10" ht="16" x14ac:dyDescent="0.2">
+      <c r="B429" s="9" t="s">
+        <v>1013</v>
+      </c>
+      <c r="C429" s="12" t="s">
+        <v>1180</v>
+      </c>
+      <c r="F429" s="10" t="s">
+        <v>832</v>
+      </c>
+      <c r="J429" s="10" t="s">
+        <v>161</v>
+      </c>
+    </row>
+    <row r="430" spans="2:10" ht="16" x14ac:dyDescent="0.2">
+      <c r="B430" s="9" t="s">
+        <v>1014</v>
+      </c>
+      <c r="C430" s="12" t="s">
+        <v>1181</v>
+      </c>
+      <c r="F430" s="10" t="s">
+        <v>812</v>
+      </c>
+      <c r="J430" s="10" t="s">
+        <v>161</v>
+      </c>
+    </row>
+    <row r="431" spans="2:10" ht="16" x14ac:dyDescent="0.2">
+      <c r="B431" s="9" t="s">
+        <v>1015</v>
+      </c>
+      <c r="C431" s="12" t="s">
+        <v>1182</v>
+      </c>
+      <c r="F431" s="10" t="s">
+        <v>812</v>
+      </c>
+      <c r="J431" s="10" t="s">
+        <v>161</v>
+      </c>
+    </row>
+    <row r="432" spans="2:10" ht="16" x14ac:dyDescent="0.2">
+      <c r="B432" s="9" t="s">
+        <v>1016</v>
+      </c>
+      <c r="C432" s="12" t="s">
+        <v>1183</v>
+      </c>
+      <c r="F432" s="10" t="s">
+        <v>812</v>
+      </c>
+      <c r="J432" s="10" t="s">
+        <v>161</v>
+      </c>
+    </row>
+    <row r="433" spans="2:10" ht="16" x14ac:dyDescent="0.2">
+      <c r="B433" s="9" t="s">
+        <v>1017</v>
+      </c>
+      <c r="C433" s="12" t="s">
+        <v>1184</v>
+      </c>
+      <c r="F433" s="10" t="s">
+        <v>812</v>
+      </c>
+      <c r="J433" s="10" t="s">
+        <v>161</v>
+      </c>
+    </row>
+    <row r="434" spans="2:10" ht="16" x14ac:dyDescent="0.2">
+      <c r="B434" s="9" t="s">
+        <v>1018</v>
+      </c>
+      <c r="C434" s="12" t="s">
+        <v>1185</v>
+      </c>
+      <c r="F434" s="10" t="s">
+        <v>812</v>
+      </c>
+      <c r="J434" s="10" t="s">
+        <v>161</v>
+      </c>
+    </row>
+    <row r="435" spans="2:10" ht="16" x14ac:dyDescent="0.2">
+      <c r="B435" s="9" t="s">
+        <v>1019</v>
+      </c>
+      <c r="C435" s="12" t="s">
+        <v>1186</v>
+      </c>
+      <c r="F435" s="10" t="s">
+        <v>812</v>
+      </c>
+      <c r="J435" s="10" t="s">
+        <v>161</v>
+      </c>
+    </row>
+    <row r="436" spans="2:10" ht="16" x14ac:dyDescent="0.2">
+      <c r="B436" s="9" t="s">
+        <v>1020</v>
+      </c>
+      <c r="C436" s="12" t="s">
+        <v>1187</v>
+      </c>
+      <c r="F436" s="10" t="s">
+        <v>812</v>
+      </c>
+      <c r="J436" s="10" t="s">
+        <v>161</v>
+      </c>
+    </row>
+    <row r="437" spans="2:10" ht="16" x14ac:dyDescent="0.2">
+      <c r="B437" s="9" t="s">
+        <v>1021</v>
+      </c>
+      <c r="C437" s="12" t="s">
+        <v>1188</v>
+      </c>
+      <c r="F437" s="10" t="s">
+        <v>812</v>
+      </c>
+      <c r="J437" s="10" t="s">
+        <v>161</v>
+      </c>
+    </row>
+    <row r="438" spans="2:10" ht="16" x14ac:dyDescent="0.2">
+      <c r="B438" s="9" t="s">
+        <v>1022</v>
+      </c>
+      <c r="C438" s="12" t="s">
+        <v>1189</v>
+      </c>
+      <c r="F438" s="10" t="s">
+        <v>812</v>
+      </c>
+      <c r="J438" s="10" t="s">
+        <v>161</v>
+      </c>
+    </row>
+    <row r="439" spans="2:10" ht="16" x14ac:dyDescent="0.2">
+      <c r="B439" s="9" t="s">
+        <v>1023</v>
+      </c>
+      <c r="C439" s="12" t="s">
+        <v>1190</v>
+      </c>
+      <c r="F439" s="10" t="s">
+        <v>812</v>
+      </c>
+      <c r="J439" s="10" t="s">
+        <v>161</v>
+      </c>
+    </row>
+    <row r="440" spans="2:10" ht="16" x14ac:dyDescent="0.2">
+      <c r="B440" s="9" t="s">
+        <v>1024</v>
+      </c>
+      <c r="C440" s="12" t="s">
+        <v>1191</v>
+      </c>
+      <c r="F440" s="10" t="s">
+        <v>812</v>
+      </c>
+      <c r="J440" s="10" t="s">
+        <v>161</v>
+      </c>
+    </row>
+    <row r="441" spans="2:10" ht="16" x14ac:dyDescent="0.2">
+      <c r="B441" s="9" t="s">
+        <v>1025</v>
+      </c>
+      <c r="C441" s="12" t="s">
+        <v>1192</v>
+      </c>
+      <c r="F441" s="10" t="s">
+        <v>812</v>
+      </c>
+      <c r="J441" s="10" t="s">
+        <v>161</v>
+      </c>
+    </row>
+    <row r="442" spans="2:10" ht="16" x14ac:dyDescent="0.2">
+      <c r="B442" s="9" t="s">
+        <v>1026</v>
+      </c>
+      <c r="C442" s="12" t="s">
+        <v>1193</v>
+      </c>
+      <c r="F442" s="10" t="s">
+        <v>812</v>
+      </c>
+      <c r="J442" s="10" t="s">
+        <v>161</v>
+      </c>
+    </row>
+    <row r="443" spans="2:10" ht="16" x14ac:dyDescent="0.2">
+      <c r="B443" s="9" t="s">
+        <v>1027</v>
+      </c>
+      <c r="C443" s="12" t="s">
+        <v>1194</v>
+      </c>
+      <c r="F443" s="10" t="s">
+        <v>812</v>
+      </c>
+      <c r="J443" s="10" t="s">
+        <v>161</v>
+      </c>
+    </row>
+    <row r="444" spans="2:10" ht="16" x14ac:dyDescent="0.2">
+      <c r="B444" s="9" t="s">
+        <v>1028</v>
+      </c>
+      <c r="C444" s="12" t="s">
+        <v>1195</v>
+      </c>
+      <c r="F444" s="10" t="s">
+        <v>851</v>
+      </c>
+      <c r="J444" s="10" t="s">
+        <v>161</v>
+      </c>
+    </row>
+    <row r="445" spans="2:10" ht="16" x14ac:dyDescent="0.2">
+      <c r="B445" s="9" t="s">
+        <v>1029</v>
+      </c>
+      <c r="C445" s="12" t="s">
+        <v>1196</v>
+      </c>
+      <c r="F445" s="10" t="s">
+        <v>52</v>
+      </c>
+      <c r="J445" s="10" t="s">
+        <v>161</v>
+      </c>
+    </row>
+    <row r="446" spans="2:10" ht="16" x14ac:dyDescent="0.2">
+      <c r="B446" s="9" t="s">
+        <v>1030</v>
+      </c>
+      <c r="C446" s="12" t="s">
+        <v>1197</v>
+      </c>
+      <c r="F446" s="10" t="s">
+        <v>812</v>
+      </c>
+      <c r="J446" s="10" t="s">
+        <v>161</v>
+      </c>
+    </row>
+    <row r="447" spans="2:10" ht="16" x14ac:dyDescent="0.2">
+      <c r="B447" s="9" t="s">
+        <v>1031</v>
+      </c>
+      <c r="C447" s="12" t="s">
+        <v>1198</v>
+      </c>
+      <c r="F447" s="10" t="s">
+        <v>812</v>
+      </c>
+      <c r="J447" s="10" t="s">
+        <v>161</v>
+      </c>
+    </row>
+    <row r="448" spans="2:10" ht="16" x14ac:dyDescent="0.2">
+      <c r="B448" s="9" t="s">
+        <v>1032</v>
+      </c>
+      <c r="C448" s="12" t="s">
+        <v>1199</v>
+      </c>
+      <c r="F448" s="10" t="s">
+        <v>812</v>
+      </c>
+      <c r="J448" s="10" t="s">
+        <v>161</v>
+      </c>
+    </row>
+    <row r="449" spans="2:10" ht="16" x14ac:dyDescent="0.2">
+      <c r="B449" s="9" t="s">
+        <v>1033</v>
+      </c>
+      <c r="C449" s="12" t="s">
+        <v>1200</v>
+      </c>
+      <c r="F449" s="10" t="s">
+        <v>812</v>
+      </c>
+      <c r="J449" s="10" t="s">
+        <v>161</v>
+      </c>
+    </row>
+    <row r="450" spans="2:10" ht="16" x14ac:dyDescent="0.2">
+      <c r="B450" s="9" t="s">
+        <v>1034</v>
+      </c>
+      <c r="C450" s="12" t="s">
+        <v>1201</v>
+      </c>
+      <c r="F450" s="10" t="s">
+        <v>812</v>
+      </c>
+      <c r="J450" s="10" t="s">
+        <v>161</v>
+      </c>
+    </row>
+    <row r="451" spans="2:10" ht="16" x14ac:dyDescent="0.2">
+      <c r="B451" s="9" t="s">
+        <v>1035</v>
+      </c>
+      <c r="C451" s="12" t="s">
+        <v>1202</v>
+      </c>
+      <c r="F451" s="10" t="s">
+        <v>812</v>
+      </c>
+      <c r="J451" s="10" t="s">
+        <v>161</v>
+      </c>
+    </row>
+    <row r="452" spans="2:10" ht="16" x14ac:dyDescent="0.2">
+      <c r="B452" s="9" t="s">
+        <v>1036</v>
+      </c>
+      <c r="C452" s="12" t="s">
+        <v>1203</v>
+      </c>
+      <c r="F452" s="10" t="s">
+        <v>812</v>
+      </c>
+      <c r="J452" s="10" t="s">
+        <v>161</v>
+      </c>
+    </row>
+    <row r="453" spans="2:10" ht="16" x14ac:dyDescent="0.2">
+      <c r="B453" s="9" t="s">
+        <v>1037</v>
+      </c>
+      <c r="C453" s="12" t="s">
+        <v>1204</v>
+      </c>
+      <c r="F453" s="10" t="s">
+        <v>812</v>
+      </c>
+      <c r="J453" s="10" t="s">
+        <v>161</v>
+      </c>
+    </row>
+    <row r="454" spans="2:10" ht="16" x14ac:dyDescent="0.2">
+      <c r="B454" s="9" t="s">
+        <v>1038</v>
+      </c>
+      <c r="C454" s="12" t="s">
+        <v>1205</v>
+      </c>
+      <c r="F454" s="10" t="s">
+        <v>812</v>
+      </c>
+      <c r="J454" s="10" t="s">
+        <v>161</v>
+      </c>
+    </row>
+    <row r="455" spans="2:10" ht="16" x14ac:dyDescent="0.2">
+      <c r="B455" s="9" t="s">
+        <v>1039</v>
+      </c>
+      <c r="C455" s="12" t="s">
+        <v>1206</v>
+      </c>
+      <c r="F455" s="10" t="s">
+        <v>812</v>
+      </c>
+      <c r="J455" s="10" t="s">
+        <v>161</v>
+      </c>
+    </row>
+    <row r="456" spans="2:10" ht="16" x14ac:dyDescent="0.2">
+      <c r="B456" s="9" t="s">
+        <v>1040</v>
+      </c>
+      <c r="C456" s="12" t="s">
+        <v>1207</v>
+      </c>
+      <c r="F456" s="9" t="s">
+        <v>811</v>
+      </c>
+      <c r="J456" s="10" t="s">
+        <v>161</v>
+      </c>
+    </row>
+    <row r="457" spans="2:10" ht="16" x14ac:dyDescent="0.2">
+      <c r="B457" s="9" t="s">
+        <v>1041</v>
+      </c>
+      <c r="C457" s="12" t="s">
+        <v>1208</v>
+      </c>
+      <c r="F457" s="9" t="s">
+        <v>856</v>
+      </c>
+      <c r="J457" s="10" t="s">
+        <v>161</v>
+      </c>
+    </row>
+    <row r="458" spans="2:10" ht="16" x14ac:dyDescent="0.2">
+      <c r="B458" s="9" t="s">
+        <v>1042</v>
+      </c>
+      <c r="C458" s="12" t="s">
+        <v>1209</v>
+      </c>
+      <c r="F458" s="10" t="s">
+        <v>812</v>
+      </c>
+      <c r="J458" s="10" t="s">
+        <v>161</v>
+      </c>
+    </row>
+    <row r="459" spans="2:10" ht="16" x14ac:dyDescent="0.2">
+      <c r="B459" s="9" t="s">
+        <v>1043</v>
+      </c>
+      <c r="C459" s="12" t="s">
+        <v>1210</v>
+      </c>
+      <c r="F459" s="10" t="s">
+        <v>812</v>
+      </c>
+      <c r="J459" s="10" t="s">
+        <v>161</v>
+      </c>
+    </row>
+    <row r="460" spans="2:10" ht="16" x14ac:dyDescent="0.2">
+      <c r="B460" s="9" t="s">
+        <v>1044</v>
+      </c>
+      <c r="C460" s="12" t="s">
+        <v>1211</v>
+      </c>
+      <c r="F460" s="10" t="s">
+        <v>812</v>
+      </c>
+      <c r="J460" s="10" t="s">
+        <v>161</v>
+      </c>
+    </row>
+    <row r="461" spans="2:10" ht="16" x14ac:dyDescent="0.2">
+      <c r="B461" s="9" t="s">
+        <v>1045</v>
+      </c>
+      <c r="C461" s="12" t="s">
+        <v>1212</v>
+      </c>
+      <c r="F461" s="10" t="s">
+        <v>52</v>
+      </c>
+      <c r="J461" s="10" t="s">
+        <v>161</v>
+      </c>
+    </row>
+    <row r="462" spans="2:10" ht="16" x14ac:dyDescent="0.2">
+      <c r="B462" s="9" t="s">
+        <v>1046</v>
+      </c>
+      <c r="C462" s="12" t="s">
+        <v>1213</v>
+      </c>
+      <c r="F462" s="10" t="s">
+        <v>851</v>
+      </c>
+      <c r="J462" s="10" t="s">
+        <v>161</v>
+      </c>
+    </row>
+    <row r="463" spans="2:10" ht="16" x14ac:dyDescent="0.2">
+      <c r="B463" s="9" t="s">
+        <v>1047</v>
+      </c>
+      <c r="C463" s="12" t="s">
+        <v>1214</v>
+      </c>
+      <c r="F463" s="10" t="s">
+        <v>851</v>
+      </c>
+      <c r="J463" s="10" t="s">
+        <v>161</v>
+      </c>
+    </row>
+    <row r="464" spans="2:10" ht="16" x14ac:dyDescent="0.2">
+      <c r="B464" s="9" t="s">
+        <v>1048</v>
+      </c>
+      <c r="C464" s="12" t="s">
+        <v>1215</v>
+      </c>
+      <c r="F464" s="10" t="s">
+        <v>831</v>
+      </c>
+      <c r="J464" s="10" t="s">
+        <v>161</v>
+      </c>
+    </row>
+    <row r="465" spans="2:10" ht="16" x14ac:dyDescent="0.2">
+      <c r="B465" s="9" t="s">
+        <v>1049</v>
+      </c>
+      <c r="C465" s="12" t="s">
+        <v>1216</v>
+      </c>
+      <c r="F465" s="10" t="s">
+        <v>811</v>
+      </c>
+      <c r="J465" s="10" t="s">
+        <v>161</v>
+      </c>
+    </row>
+    <row r="466" spans="2:10" ht="16" x14ac:dyDescent="0.2">
+      <c r="B466" s="9" t="s">
+        <v>1050</v>
+      </c>
+      <c r="C466" s="12" t="s">
+        <v>1217</v>
+      </c>
+      <c r="F466" s="10" t="s">
+        <v>831</v>
+      </c>
+      <c r="J466" s="10" t="s">
+        <v>161</v>
+      </c>
+    </row>
+    <row r="467" spans="2:10" ht="16" x14ac:dyDescent="0.2">
+      <c r="B467" s="9" t="s">
+        <v>1051</v>
+      </c>
+      <c r="C467" s="12" t="s">
+        <v>1218</v>
+      </c>
+      <c r="F467" s="10" t="s">
+        <v>831</v>
+      </c>
+      <c r="J467" s="10" t="s">
+        <v>161</v>
+      </c>
+    </row>
+    <row r="468" spans="2:10" ht="16" x14ac:dyDescent="0.2">
+      <c r="B468" s="9" t="s">
+        <v>1052</v>
+      </c>
+      <c r="C468" s="12" t="s">
+        <v>1219</v>
+      </c>
+      <c r="F468" s="10" t="s">
+        <v>812</v>
+      </c>
+      <c r="J468" s="10" t="s">
+        <v>161</v>
+      </c>
+    </row>
+    <row r="469" spans="2:10" ht="16" x14ac:dyDescent="0.2">
+      <c r="B469" s="9" t="s">
+        <v>1053</v>
+      </c>
+      <c r="C469" s="12" t="s">
+        <v>1220</v>
+      </c>
+      <c r="F469" s="10" t="s">
+        <v>812</v>
+      </c>
+      <c r="J469" s="10" t="s">
+        <v>161</v>
+      </c>
+    </row>
+    <row r="470" spans="2:10" ht="16" x14ac:dyDescent="0.2">
+      <c r="B470" s="9" t="s">
+        <v>1054</v>
+      </c>
+      <c r="C470" s="12" t="s">
+        <v>1224</v>
+      </c>
+      <c r="F470" s="10" t="s">
+        <v>812</v>
+      </c>
+      <c r="J470" s="10" t="s">
+        <v>161</v>
+      </c>
+    </row>
+    <row r="471" spans="2:10" ht="16" x14ac:dyDescent="0.2">
+      <c r="B471" s="9" t="s">
+        <v>1055</v>
+      </c>
+      <c r="C471" s="12" t="s">
+        <v>1230</v>
+      </c>
+      <c r="F471" s="10" t="s">
+        <v>812</v>
+      </c>
+      <c r="J471" s="10" t="s">
+        <v>161</v>
+      </c>
+    </row>
+    <row r="472" spans="2:10" ht="16" x14ac:dyDescent="0.2">
+      <c r="B472" s="9" t="s">
+        <v>1056</v>
+      </c>
+      <c r="C472" s="12" t="s">
+        <v>1221</v>
+      </c>
+      <c r="F472" s="10" t="s">
+        <v>812</v>
+      </c>
+      <c r="J472" s="10" t="s">
+        <v>161</v>
+      </c>
+    </row>
+    <row r="473" spans="2:10" ht="16" x14ac:dyDescent="0.2">
+      <c r="B473" s="9" t="s">
+        <v>1057</v>
+      </c>
+      <c r="C473" s="12" t="s">
+        <v>1222</v>
+      </c>
+      <c r="F473" s="10" t="s">
+        <v>812</v>
+      </c>
+      <c r="J473" s="10" t="s">
+        <v>161</v>
+      </c>
+    </row>
+    <row r="474" spans="2:10" ht="16" x14ac:dyDescent="0.2">
+      <c r="B474" s="9" t="s">
+        <v>1058</v>
+      </c>
+      <c r="C474" s="12" t="s">
+        <v>1223</v>
+      </c>
+      <c r="F474" s="10" t="s">
+        <v>812</v>
+      </c>
+      <c r="J474" s="10" t="s">
+        <v>161</v>
+      </c>
+    </row>
+    <row r="475" spans="2:10" ht="16" x14ac:dyDescent="0.2">
+      <c r="B475" s="9" t="s">
+        <v>1059</v>
+      </c>
+      <c r="C475" s="12" t="s">
+        <v>1225</v>
+      </c>
+      <c r="F475" s="10" t="s">
+        <v>812</v>
+      </c>
+      <c r="J475" s="10" t="s">
+        <v>161</v>
+      </c>
+    </row>
+    <row r="476" spans="2:10" ht="16" x14ac:dyDescent="0.2">
+      <c r="B476" s="9" t="s">
+        <v>1060</v>
+      </c>
+      <c r="C476" s="12" t="s">
+        <v>1226</v>
+      </c>
+      <c r="F476" s="10" t="s">
+        <v>812</v>
+      </c>
+      <c r="J476" s="10" t="s">
+        <v>161</v>
+      </c>
+    </row>
+    <row r="477" spans="2:10" ht="16" x14ac:dyDescent="0.2">
+      <c r="B477" s="9" t="s">
+        <v>1061</v>
+      </c>
+      <c r="C477" s="12" t="s">
+        <v>1227</v>
+      </c>
+      <c r="F477" s="10" t="s">
+        <v>812</v>
+      </c>
+      <c r="J477" s="10" t="s">
+        <v>161</v>
+      </c>
+    </row>
+    <row r="478" spans="2:10" ht="16" x14ac:dyDescent="0.2">
+      <c r="B478" s="9" t="s">
+        <v>1062</v>
+      </c>
+      <c r="C478" s="12" t="s">
+        <v>1228</v>
+      </c>
+      <c r="F478" s="10" t="s">
+        <v>812</v>
+      </c>
+      <c r="J478" s="10" t="s">
+        <v>161</v>
+      </c>
+    </row>
+    <row r="479" spans="2:10" ht="16" x14ac:dyDescent="0.2">
+      <c r="B479" s="9" t="s">
+        <v>1063</v>
+      </c>
+      <c r="C479" s="12" t="s">
+        <v>1229</v>
+      </c>
+      <c r="F479" s="10" t="s">
+        <v>812</v>
+      </c>
+      <c r="J479" s="10" t="s">
+        <v>161</v>
+      </c>
+    </row>
+    <row r="480" spans="2:10" ht="16" x14ac:dyDescent="0.2">
+      <c r="B480" s="9" t="s">
+        <v>1064</v>
+      </c>
+      <c r="C480" s="12" t="s">
+        <v>1231</v>
+      </c>
+      <c r="F480" s="10" t="s">
+        <v>812</v>
+      </c>
+      <c r="J480" s="10" t="s">
+        <v>161</v>
+      </c>
+    </row>
+    <row r="481" spans="2:10" ht="16" x14ac:dyDescent="0.2">
+      <c r="B481" s="9" t="s">
+        <v>1065</v>
+      </c>
+      <c r="C481" s="12" t="s">
+        <v>1232</v>
+      </c>
+      <c r="F481" s="10" t="s">
+        <v>812</v>
+      </c>
+      <c r="J481" s="10" t="s">
+        <v>161</v>
+      </c>
+    </row>
+    <row r="482" spans="2:10" ht="16" x14ac:dyDescent="0.2">
+      <c r="B482" s="9" t="s">
+        <v>1066</v>
+      </c>
+      <c r="C482" s="12" t="s">
+        <v>1233</v>
+      </c>
+      <c r="F482" s="10" t="s">
+        <v>812</v>
+      </c>
+      <c r="J482" s="10" t="s">
+        <v>161</v>
+      </c>
+    </row>
+    <row r="483" spans="2:10" ht="16" x14ac:dyDescent="0.2">
+      <c r="B483" s="9" t="s">
+        <v>1067</v>
+      </c>
+      <c r="C483" s="12" t="s">
+        <v>1234</v>
+      </c>
+      <c r="F483" s="10" t="s">
+        <v>812</v>
+      </c>
+      <c r="J483" s="10" t="s">
+        <v>161</v>
+      </c>
+    </row>
+    <row r="484" spans="2:10" ht="16" x14ac:dyDescent="0.2">
+      <c r="B484" s="9" t="s">
+        <v>1068</v>
+      </c>
+      <c r="C484" s="12" t="s">
+        <v>1235</v>
+      </c>
+      <c r="F484" s="10" t="s">
+        <v>812</v>
+      </c>
+      <c r="J484" s="10" t="s">
+        <v>161</v>
+      </c>
+    </row>
+    <row r="485" spans="2:10" ht="16" x14ac:dyDescent="0.2">
+      <c r="B485" s="9" t="s">
+        <v>1069</v>
+      </c>
+      <c r="C485" s="12" t="s">
+        <v>1236</v>
+      </c>
+      <c r="F485" s="10" t="s">
+        <v>812</v>
+      </c>
+      <c r="J485" s="10" t="s">
+        <v>161</v>
+      </c>
+    </row>
+    <row r="486" spans="2:10" x14ac:dyDescent="0.15">
+      <c r="B486" s="9" t="s">
+        <v>1070</v>
+      </c>
+      <c r="C486" s="13" t="s">
+        <v>1237</v>
+      </c>
+      <c r="F486" s="10" t="s">
+        <v>812</v>
+      </c>
+      <c r="J486" s="10" t="s">
+        <v>162</v>
+      </c>
+    </row>
+    <row r="487" spans="2:10" x14ac:dyDescent="0.15">
+      <c r="B487" s="9" t="s">
+        <v>1071</v>
+      </c>
+      <c r="C487" s="13" t="s">
+        <v>1238</v>
+      </c>
+      <c r="F487" s="10" t="s">
+        <v>811</v>
+      </c>
+      <c r="J487" s="10" t="s">
+        <v>162</v>
+      </c>
+    </row>
+    <row r="488" spans="2:10" x14ac:dyDescent="0.15">
+      <c r="B488" s="9" t="s">
+        <v>1072</v>
+      </c>
+      <c r="C488" s="13" t="s">
+        <v>1239</v>
+      </c>
+      <c r="F488" s="10" t="s">
+        <v>811</v>
+      </c>
+      <c r="J488" s="10" t="s">
+        <v>162</v>
+      </c>
+    </row>
+    <row r="489" spans="2:10" x14ac:dyDescent="0.15">
+      <c r="B489" s="9" t="s">
+        <v>1073</v>
+      </c>
+      <c r="C489" s="13" t="s">
+        <v>1240</v>
+      </c>
+      <c r="F489" s="10" t="s">
+        <v>811</v>
+      </c>
+      <c r="J489" s="10" t="s">
+        <v>161</v>
+      </c>
+    </row>
+    <row r="490" spans="2:10" x14ac:dyDescent="0.15">
+      <c r="B490" s="9" t="s">
+        <v>1074</v>
+      </c>
+      <c r="C490" s="13" t="s">
+        <v>1241</v>
+      </c>
+      <c r="F490" s="10" t="s">
+        <v>811</v>
+      </c>
+      <c r="J490" s="10" t="s">
+        <v>162</v>
+      </c>
+    </row>
+    <row r="491" spans="2:10" x14ac:dyDescent="0.15">
+      <c r="B491" s="9" t="s">
+        <v>1075</v>
+      </c>
+      <c r="C491" s="13" t="s">
+        <v>1242</v>
+      </c>
+      <c r="F491" s="10" t="s">
+        <v>811</v>
+      </c>
+      <c r="J491" s="10" t="s">
+        <v>161</v>
+      </c>
+    </row>
+    <row r="492" spans="2:10" x14ac:dyDescent="0.15">
+      <c r="B492" s="9" t="s">
+        <v>1076</v>
+      </c>
+      <c r="C492" s="13" t="s">
+        <v>1243</v>
+      </c>
+      <c r="F492" s="10" t="s">
+        <v>811</v>
+      </c>
+      <c r="J492" s="10" t="s">
+        <v>162</v>
+      </c>
+    </row>
+    <row r="493" spans="2:10" x14ac:dyDescent="0.15">
+      <c r="B493" s="9" t="s">
+        <v>1077</v>
+      </c>
+      <c r="C493" s="13" t="s">
+        <v>1244</v>
+      </c>
+      <c r="F493" s="10" t="s">
+        <v>811</v>
+      </c>
+      <c r="J493" s="10" t="s">
+        <v>161</v>
+      </c>
+    </row>
+    <row r="494" spans="2:10" x14ac:dyDescent="0.15">
+      <c r="B494" s="9" t="s">
+        <v>1078</v>
+      </c>
+      <c r="C494" s="13" t="s">
+        <v>1245</v>
+      </c>
+      <c r="F494" s="10" t="s">
+        <v>811</v>
+      </c>
+      <c r="J494" s="10" t="s">
+        <v>162</v>
+      </c>
+    </row>
+    <row r="495" spans="2:10" x14ac:dyDescent="0.15">
+      <c r="B495" s="9" t="s">
+        <v>1079</v>
+      </c>
+      <c r="C495" s="13" t="s">
+        <v>1246</v>
+      </c>
+      <c r="F495" s="10" t="s">
+        <v>811</v>
+      </c>
+      <c r="J495" s="10" t="s">
+        <v>161</v>
+      </c>
+    </row>
+    <row r="496" spans="2:10" x14ac:dyDescent="0.15">
+      <c r="B496" s="9" t="s">
+        <v>1080</v>
+      </c>
+      <c r="C496" s="13" t="s">
+        <v>1247</v>
+      </c>
+      <c r="F496" s="10" t="s">
+        <v>811</v>
+      </c>
+      <c r="J496" s="10" t="s">
+        <v>162</v>
+      </c>
+    </row>
+    <row r="497" spans="2:10" x14ac:dyDescent="0.15">
+      <c r="B497" s="9" t="s">
+        <v>1081</v>
+      </c>
+      <c r="C497" s="13" t="s">
+        <v>1248</v>
+      </c>
+      <c r="F497" s="10" t="s">
+        <v>811</v>
+      </c>
+      <c r="J497" s="10" t="s">
+        <v>161</v>
+      </c>
+    </row>
+    <row r="498" spans="2:10" x14ac:dyDescent="0.15">
+      <c r="B498" s="9" t="s">
+        <v>1082</v>
+      </c>
+      <c r="C498" s="13" t="s">
+        <v>1249</v>
+      </c>
+      <c r="F498" s="10" t="s">
+        <v>811</v>
+      </c>
+      <c r="J498" s="10" t="s">
+        <v>162</v>
+      </c>
+    </row>
+    <row r="499" spans="2:10" x14ac:dyDescent="0.15">
+      <c r="B499" s="9" t="s">
+        <v>1083</v>
+      </c>
+      <c r="C499" s="13" t="s">
+        <v>1250</v>
+      </c>
+      <c r="F499" s="10" t="s">
+        <v>811</v>
+      </c>
+      <c r="J499" s="10" t="s">
+        <v>161</v>
+      </c>
+    </row>
+    <row r="500" spans="2:10" x14ac:dyDescent="0.15">
+      <c r="B500" s="9" t="s">
+        <v>1084</v>
+      </c>
+      <c r="C500" s="13" t="s">
+        <v>1251</v>
+      </c>
+      <c r="F500" s="10" t="s">
+        <v>811</v>
+      </c>
+      <c r="J500" s="10" t="s">
+        <v>162</v>
+      </c>
+    </row>
+    <row r="501" spans="2:10" x14ac:dyDescent="0.15">
+      <c r="B501" s="9" t="s">
+        <v>1085</v>
+      </c>
+      <c r="C501" s="13" t="s">
+        <v>1252</v>
+      </c>
+      <c r="F501" s="10" t="s">
+        <v>811</v>
+      </c>
+      <c r="J501" s="10" t="s">
+        <v>161</v>
+      </c>
+    </row>
+    <row r="502" spans="2:10" x14ac:dyDescent="0.15">
+      <c r="B502" s="9" t="s">
+        <v>1086</v>
+      </c>
+      <c r="C502" s="13" t="s">
+        <v>1253</v>
+      </c>
+      <c r="F502" s="10" t="s">
+        <v>811</v>
+      </c>
+      <c r="J502" s="10" t="s">
+        <v>162</v>
+      </c>
+    </row>
+    <row r="503" spans="2:10" x14ac:dyDescent="0.15">
+      <c r="B503" s="9" t="s">
+        <v>1087</v>
+      </c>
+      <c r="C503" s="13" t="s">
+        <v>1254</v>
+      </c>
+      <c r="F503" s="10" t="s">
+        <v>811</v>
+      </c>
+      <c r="J503" s="10" t="s">
+        <v>161</v>
+      </c>
+    </row>
+    <row r="504" spans="2:10" x14ac:dyDescent="0.15">
+      <c r="B504" s="9" t="s">
+        <v>1088</v>
+      </c>
+      <c r="C504" s="13" t="s">
+        <v>1255</v>
+      </c>
+      <c r="F504" s="10" t="s">
+        <v>811</v>
+      </c>
+      <c r="J504" s="10" t="s">
+        <v>162</v>
+      </c>
+    </row>
+    <row r="505" spans="2:10" x14ac:dyDescent="0.15">
+      <c r="B505" s="9" t="s">
+        <v>1089</v>
+      </c>
+      <c r="C505" s="13" t="s">
+        <v>1256</v>
+      </c>
+      <c r="F505" s="10" t="s">
+        <v>811</v>
+      </c>
+      <c r="J505" s="10" t="s">
+        <v>161</v>
+      </c>
+    </row>
+    <row r="506" spans="2:10" x14ac:dyDescent="0.15">
+      <c r="B506" s="9" t="s">
+        <v>1090</v>
+      </c>
+      <c r="C506" s="13" t="s">
+        <v>1257</v>
+      </c>
+      <c r="F506" s="10" t="s">
+        <v>811</v>
+      </c>
+      <c r="J506" s="10" t="s">
+        <v>162</v>
+      </c>
+    </row>
+    <row r="507" spans="2:10" x14ac:dyDescent="0.15">
+      <c r="B507" s="9" t="s">
+        <v>1091</v>
+      </c>
+      <c r="C507" s="13" t="s">
+        <v>1258</v>
+      </c>
+      <c r="F507" s="10" t="s">
+        <v>811</v>
+      </c>
+      <c r="J507" s="10" t="s">
+        <v>161</v>
+      </c>
+    </row>
+    <row r="508" spans="2:10" x14ac:dyDescent="0.15">
+      <c r="B508" s="9" t="s">
+        <v>1092</v>
+      </c>
+      <c r="C508" s="13" t="s">
+        <v>1259</v>
+      </c>
+      <c r="F508" s="10" t="s">
+        <v>811</v>
+      </c>
+      <c r="J508" s="10" t="s">
+        <v>162</v>
+      </c>
+    </row>
+    <row r="509" spans="2:10" x14ac:dyDescent="0.15">
+      <c r="B509" s="9" t="s">
+        <v>1093</v>
+      </c>
+      <c r="C509" s="13" t="s">
+        <v>1260</v>
+      </c>
+      <c r="F509" s="10" t="s">
+        <v>811</v>
+      </c>
+      <c r="J509" s="10" t="s">
+        <v>161</v>
+      </c>
+    </row>
+    <row r="510" spans="2:10" x14ac:dyDescent="0.15">
+      <c r="B510" s="9" t="s">
+        <v>1094</v>
+      </c>
+      <c r="C510" s="13" t="s">
+        <v>1261</v>
+      </c>
+      <c r="F510" s="10" t="s">
+        <v>811</v>
+      </c>
+      <c r="J510" s="10" t="s">
+        <v>162</v>
+      </c>
+    </row>
+    <row r="511" spans="2:10" x14ac:dyDescent="0.15">
+      <c r="B511" s="9" t="s">
+        <v>1095</v>
+      </c>
+      <c r="C511" s="13" t="s">
+        <v>1262</v>
+      </c>
+      <c r="F511" s="10" t="s">
+        <v>811</v>
+      </c>
+      <c r="J511" s="10" t="s">
+        <v>162</v>
+      </c>
+    </row>
+    <row r="512" spans="2:10" x14ac:dyDescent="0.15">
+      <c r="B512" s="9" t="s">
+        <v>1096</v>
+      </c>
+      <c r="C512" s="13" t="s">
+        <v>1263</v>
+      </c>
+      <c r="F512" s="10" t="s">
+        <v>811</v>
+      </c>
+      <c r="J512" s="10" t="s">
+        <v>161</v>
+      </c>
+    </row>
+    <row r="513" spans="2:10" x14ac:dyDescent="0.15">
+      <c r="B513" s="9" t="s">
+        <v>1097</v>
+      </c>
+      <c r="C513" s="13" t="s">
+        <v>1264</v>
+      </c>
+      <c r="F513" s="10" t="s">
+        <v>811</v>
+      </c>
+      <c r="J513" s="10" t="s">
+        <v>162</v>
+      </c>
+    </row>
+    <row r="514" spans="2:10" x14ac:dyDescent="0.15">
+      <c r="B514" s="9" t="s">
+        <v>1098</v>
+      </c>
+      <c r="C514" s="13" t="s">
+        <v>1265</v>
+      </c>
+      <c r="F514" s="10" t="s">
+        <v>811</v>
+      </c>
+      <c r="J514" s="10" t="s">
+        <v>161</v>
+      </c>
+    </row>
+    <row r="515" spans="2:10" x14ac:dyDescent="0.15">
+      <c r="B515" s="9" t="s">
+        <v>1099</v>
+      </c>
+      <c r="C515" s="13" t="s">
+        <v>1266</v>
+      </c>
+      <c r="F515" s="10" t="s">
+        <v>811</v>
+      </c>
+      <c r="J515" s="10" t="s">
+        <v>162</v>
+      </c>
+    </row>
+    <row r="516" spans="2:10" x14ac:dyDescent="0.15">
+      <c r="B516" s="9" t="s">
+        <v>1100</v>
+      </c>
+      <c r="C516" s="13" t="s">
+        <v>1267</v>
+      </c>
+      <c r="F516" s="10" t="s">
+        <v>811</v>
+      </c>
+      <c r="J516" s="10" t="s">
+        <v>161</v>
+      </c>
+    </row>
+    <row r="517" spans="2:10" x14ac:dyDescent="0.15">
+      <c r="B517" s="9" t="s">
+        <v>1101</v>
+      </c>
+      <c r="C517" s="13" t="s">
+        <v>1268</v>
+      </c>
+      <c r="F517" s="10" t="s">
+        <v>811</v>
+      </c>
+      <c r="J517" s="10" t="s">
+        <v>162</v>
+      </c>
+    </row>
+    <row r="518" spans="2:10" x14ac:dyDescent="0.15">
+      <c r="B518" s="9" t="s">
+        <v>1102</v>
+      </c>
+      <c r="C518" s="13" t="s">
+        <v>1269</v>
+      </c>
+      <c r="F518" s="10" t="s">
+        <v>811</v>
+      </c>
+      <c r="J518" s="10" t="s">
+        <v>161</v>
+      </c>
+    </row>
+    <row r="519" spans="2:10" x14ac:dyDescent="0.15">
+      <c r="B519" s="9" t="s">
+        <v>1103</v>
+      </c>
+      <c r="C519" s="13" t="s">
+        <v>1270</v>
+      </c>
+      <c r="F519" s="10" t="s">
+        <v>811</v>
+      </c>
+      <c r="J519" s="10" t="s">
+        <v>162</v>
+      </c>
+    </row>
+    <row r="520" spans="2:10" x14ac:dyDescent="0.15">
+      <c r="B520" s="9" t="s">
+        <v>1104</v>
+      </c>
+      <c r="C520" s="13" t="s">
+        <v>1271</v>
+      </c>
+      <c r="F520" s="10" t="s">
+        <v>811</v>
+      </c>
+      <c r="J520" s="10" t="s">
+        <v>161</v>
+      </c>
+    </row>
+    <row r="521" spans="2:10" x14ac:dyDescent="0.15">
+      <c r="B521" s="9" t="s">
+        <v>1105</v>
+      </c>
+      <c r="C521" s="13" t="s">
+        <v>1272</v>
+      </c>
+      <c r="F521" s="10" t="s">
+        <v>811</v>
+      </c>
+      <c r="J521" s="10" t="s">
+        <v>162</v>
+      </c>
+    </row>
+    <row r="522" spans="2:10" x14ac:dyDescent="0.15">
+      <c r="B522" s="9" t="s">
+        <v>1106</v>
+      </c>
+      <c r="C522" s="13" t="s">
+        <v>1273</v>
+      </c>
+      <c r="F522" s="10" t="s">
+        <v>811</v>
+      </c>
+      <c r="J522" s="10" t="s">
+        <v>161</v>
+      </c>
+    </row>
+    <row r="523" spans="2:10" x14ac:dyDescent="0.15">
+      <c r="B523" s="9" t="s">
+        <v>1107</v>
+      </c>
+      <c r="C523" s="13" t="s">
+        <v>1274</v>
+      </c>
+      <c r="F523" s="10" t="s">
+        <v>811</v>
+      </c>
+      <c r="J523" s="10" t="s">
+        <v>162</v>
+      </c>
+    </row>
+    <row r="524" spans="2:10" x14ac:dyDescent="0.15">
+      <c r="B524" s="9" t="s">
+        <v>1108</v>
+      </c>
+      <c r="C524" s="13" t="s">
+        <v>1275</v>
+      </c>
+      <c r="F524" s="10" t="s">
+        <v>811</v>
+      </c>
+      <c r="J524" s="10" t="s">
+        <v>161</v>
+      </c>
+    </row>
+    <row r="525" spans="2:10" x14ac:dyDescent="0.15">
+      <c r="B525" s="9" t="s">
+        <v>1109</v>
+      </c>
+      <c r="C525" s="13" t="s">
+        <v>1276</v>
+      </c>
+      <c r="F525" s="10" t="s">
+        <v>811</v>
+      </c>
+      <c r="J525" s="10" t="s">
+        <v>162</v>
+      </c>
+    </row>
+    <row r="526" spans="2:10" x14ac:dyDescent="0.15">
+      <c r="B526" s="9" t="s">
+        <v>1110</v>
+      </c>
+      <c r="C526" s="13" t="s">
+        <v>1277</v>
+      </c>
+      <c r="F526" s="10" t="s">
+        <v>811</v>
+      </c>
+      <c r="J526" s="10" t="s">
+        <v>161</v>
+      </c>
+    </row>
+    <row r="527" spans="2:10" x14ac:dyDescent="0.15">
+      <c r="B527" s="9" t="s">
+        <v>1111</v>
+      </c>
+      <c r="C527" s="13" t="s">
+        <v>1278</v>
+      </c>
+      <c r="F527" s="10" t="s">
+        <v>811</v>
+      </c>
+      <c r="J527" s="10" t="s">
+        <v>162</v>
+      </c>
+    </row>
+    <row r="528" spans="2:10" x14ac:dyDescent="0.15">
+      <c r="B528" s="9" t="s">
+        <v>1112</v>
+      </c>
+      <c r="C528" s="13" t="s">
+        <v>1279</v>
+      </c>
+      <c r="F528" s="10" t="s">
+        <v>811</v>
+      </c>
+      <c r="J528" s="10" t="s">
+        <v>161</v>
+      </c>
+    </row>
+    <row r="529" spans="2:10" x14ac:dyDescent="0.15">
+      <c r="B529" s="9" t="s">
+        <v>1113</v>
+      </c>
+      <c r="C529" s="13" t="s">
+        <v>1280</v>
+      </c>
+      <c r="F529" s="10" t="s">
+        <v>811</v>
+      </c>
+      <c r="J529" s="10" t="s">
+        <v>161</v>
+      </c>
+    </row>
+    <row r="530" spans="2:10" x14ac:dyDescent="0.15">
+      <c r="B530" s="9" t="s">
+        <v>1114</v>
+      </c>
+      <c r="C530" s="13" t="s">
+        <v>1281</v>
+      </c>
+      <c r="F530" s="10" t="s">
+        <v>811</v>
+      </c>
+      <c r="J530" s="10" t="s">
+        <v>161</v>
+      </c>
+    </row>
+    <row r="531" spans="2:10" x14ac:dyDescent="0.15">
+      <c r="B531" s="9" t="s">
+        <v>1115</v>
+      </c>
+      <c r="C531" s="13" t="s">
+        <v>1282</v>
+      </c>
+      <c r="F531" s="10" t="s">
+        <v>811</v>
+      </c>
+      <c r="J531" s="10" t="s">
+        <v>161</v>
+      </c>
+    </row>
+    <row r="532" spans="2:10" x14ac:dyDescent="0.15">
+      <c r="B532" s="9" t="s">
+        <v>1116</v>
+      </c>
+      <c r="C532" s="13" t="s">
+        <v>1283</v>
+      </c>
+      <c r="F532" s="10" t="s">
+        <v>811</v>
+      </c>
+      <c r="J532" s="10" t="s">
+        <v>161</v>
+      </c>
+    </row>
+    <row r="533" spans="2:10" x14ac:dyDescent="0.15">
+      <c r="B533" s="9" t="s">
+        <v>1117</v>
+      </c>
+      <c r="C533" s="13" t="s">
+        <v>1284</v>
+      </c>
+      <c r="F533" s="10" t="s">
+        <v>811</v>
+      </c>
+      <c r="J533" s="10" t="s">
+        <v>161</v>
+      </c>
+    </row>
+    <row r="534" spans="2:10" x14ac:dyDescent="0.15">
+      <c r="B534" s="9" t="s">
+        <v>1118</v>
+      </c>
+      <c r="C534" s="13" t="s">
+        <v>1285</v>
+      </c>
+      <c r="F534" s="10" t="s">
+        <v>811</v>
+      </c>
+      <c r="J534" s="10" t="s">
+        <v>161</v>
+      </c>
+    </row>
+    <row r="535" spans="2:10" x14ac:dyDescent="0.15">
+      <c r="B535" s="9" t="s">
+        <v>1119</v>
+      </c>
+      <c r="C535" s="13" t="s">
+        <v>1286</v>
+      </c>
+      <c r="F535" s="10" t="s">
+        <v>811</v>
+      </c>
+      <c r="J535" s="10" t="s">
+        <v>161</v>
+      </c>
+    </row>
+    <row r="536" spans="2:10" x14ac:dyDescent="0.15">
+      <c r="B536" s="9" t="s">
+        <v>1120</v>
+      </c>
+      <c r="C536" s="13" t="s">
+        <v>1287</v>
+      </c>
+      <c r="F536" s="10" t="s">
+        <v>811</v>
+      </c>
+      <c r="J536" s="10" t="s">
+        <v>161</v>
+      </c>
+    </row>
+    <row r="537" spans="2:10" x14ac:dyDescent="0.15">
+      <c r="B537" s="9" t="s">
+        <v>1121</v>
+      </c>
+      <c r="C537" s="13" t="s">
+        <v>1288</v>
+      </c>
+      <c r="F537" s="10" t="s">
+        <v>811</v>
+      </c>
+      <c r="J537" s="10" t="s">
+        <v>161</v>
+      </c>
+    </row>
+    <row r="538" spans="2:10" x14ac:dyDescent="0.15">
+      <c r="B538" s="9" t="s">
+        <v>1122</v>
+      </c>
+      <c r="C538" s="13" t="s">
+        <v>1289</v>
+      </c>
+      <c r="F538" s="10" t="s">
+        <v>811</v>
+      </c>
+      <c r="J538" s="10" t="s">
+        <v>161</v>
+      </c>
+    </row>
+    <row r="539" spans="2:10" x14ac:dyDescent="0.15">
+      <c r="B539" s="9" t="s">
+        <v>1123</v>
+      </c>
+      <c r="C539" s="13" t="s">
+        <v>1290</v>
+      </c>
+      <c r="F539" s="10" t="s">
+        <v>811</v>
+      </c>
+      <c r="J539" s="10" t="s">
+        <v>161</v>
+      </c>
+    </row>
+    <row r="540" spans="2:10" x14ac:dyDescent="0.15">
+      <c r="B540" s="9" t="s">
+        <v>1124</v>
+      </c>
+      <c r="C540" s="13" t="s">
+        <v>1291</v>
+      </c>
+      <c r="F540" s="10" t="s">
+        <v>811</v>
+      </c>
+      <c r="J540" s="10" t="s">
+        <v>161</v>
+      </c>
+    </row>
+    <row r="541" spans="2:10" x14ac:dyDescent="0.15">
+      <c r="B541" s="9" t="s">
+        <v>1125</v>
+      </c>
+      <c r="C541" s="13" t="s">
+        <v>1292</v>
+      </c>
+      <c r="F541" s="10" t="s">
+        <v>811</v>
+      </c>
+      <c r="J541" s="10" t="s">
+        <v>161</v>
+      </c>
+    </row>
+    <row r="542" spans="2:10" x14ac:dyDescent="0.15">
+      <c r="B542" s="9" t="s">
+        <v>1126</v>
+      </c>
+      <c r="C542" s="13" t="s">
+        <v>1293</v>
+      </c>
+      <c r="F542" s="10" t="s">
+        <v>811</v>
+      </c>
+      <c r="J542" s="10" t="s">
+        <v>161</v>
+      </c>
+    </row>
+    <row r="543" spans="2:10" x14ac:dyDescent="0.15">
+      <c r="B543" s="9" t="s">
+        <v>1127</v>
+      </c>
+      <c r="C543" s="13" t="s">
+        <v>1294</v>
+      </c>
+      <c r="F543" s="10" t="s">
+        <v>811</v>
+      </c>
+      <c r="J543" s="10" t="s">
+        <v>161</v>
+      </c>
+    </row>
+    <row r="544" spans="2:10" x14ac:dyDescent="0.15">
+      <c r="B544" s="9" t="s">
+        <v>1128</v>
+      </c>
+      <c r="C544" s="13" t="s">
+        <v>1295</v>
+      </c>
+      <c r="F544" s="10" t="s">
+        <v>811</v>
+      </c>
+      <c r="J544" s="10" t="s">
+        <v>161</v>
+      </c>
+    </row>
+    <row r="545" spans="2:10" x14ac:dyDescent="0.15">
+      <c r="B545" s="9" t="s">
+        <v>1129</v>
+      </c>
+      <c r="C545" s="13" t="s">
+        <v>1296</v>
+      </c>
+      <c r="F545" s="10" t="s">
+        <v>811</v>
+      </c>
+      <c r="J545" s="10" t="s">
+        <v>161</v>
+      </c>
+    </row>
+    <row r="546" spans="2:10" x14ac:dyDescent="0.15">
+      <c r="B546" s="9" t="s">
+        <v>1130</v>
+      </c>
+      <c r="C546" s="13" t="s">
+        <v>1297</v>
+      </c>
+      <c r="F546" s="10" t="s">
+        <v>811</v>
+      </c>
+      <c r="J546" s="10" t="s">
+        <v>161</v>
+      </c>
+    </row>
+    <row r="547" spans="2:10" x14ac:dyDescent="0.15">
+      <c r="B547" s="9" t="s">
+        <v>1131</v>
+      </c>
+      <c r="C547" s="13" t="s">
+        <v>1298</v>
+      </c>
+      <c r="F547" s="10" t="s">
+        <v>811</v>
+      </c>
+      <c r="J547" s="10" t="s">
+        <v>161</v>
+      </c>
+    </row>
+    <row r="548" spans="2:10" x14ac:dyDescent="0.15">
+      <c r="B548" s="9" t="s">
+        <v>1132</v>
+      </c>
+      <c r="C548" s="10" t="s">
+        <v>1299</v>
+      </c>
+      <c r="F548" s="10" t="s">
+        <v>831</v>
+      </c>
+      <c r="J548" s="10" t="s">
+        <v>161</v>
+      </c>
+    </row>
+    <row r="549" spans="2:10" x14ac:dyDescent="0.15">
+      <c r="B549" s="9" t="s">
+        <v>1133</v>
+      </c>
+      <c r="C549" s="10" t="s">
+        <v>1300</v>
+      </c>
+      <c r="F549" s="10" t="s">
+        <v>851</v>
+      </c>
+      <c r="J549" s="10" t="s">
+        <v>161</v>
+      </c>
+    </row>
+    <row r="550" spans="2:10" x14ac:dyDescent="0.15">
+      <c r="B550" s="9" t="s">
+        <v>1134</v>
+      </c>
+      <c r="C550" s="10" t="s">
+        <v>1301</v>
+      </c>
+      <c r="F550" s="10" t="s">
+        <v>851</v>
+      </c>
+      <c r="J550" s="10" t="s">
+        <v>161</v>
+      </c>
+    </row>
+    <row r="551" spans="2:10" x14ac:dyDescent="0.15">
+      <c r="B551" s="9" t="s">
+        <v>1135</v>
+      </c>
+      <c r="C551" s="10" t="s">
+        <v>1302</v>
+      </c>
+      <c r="F551" s="10" t="s">
+        <v>851</v>
+      </c>
+      <c r="J551" s="10" t="s">
+        <v>161</v>
+      </c>
+    </row>
+    <row r="552" spans="2:10" x14ac:dyDescent="0.15">
+      <c r="B552" s="9" t="s">
+        <v>1136</v>
+      </c>
+      <c r="C552" s="10" t="s">
+        <v>1303</v>
+      </c>
+      <c r="F552" s="10" t="s">
+        <v>851</v>
+      </c>
+      <c r="J552" s="10" t="s">
+        <v>161</v>
+      </c>
+    </row>
+    <row r="553" spans="2:10" x14ac:dyDescent="0.15">
+      <c r="B553" s="9" t="s">
+        <v>1137</v>
+      </c>
+      <c r="C553" s="10" t="s">
+        <v>1304</v>
+      </c>
+      <c r="F553" s="10" t="s">
+        <v>829</v>
+      </c>
+      <c r="J553" s="10" t="s">
+        <v>161</v>
+      </c>
+    </row>
+    <row r="554" spans="2:10" x14ac:dyDescent="0.15">
+      <c r="B554" s="9" t="s">
+        <v>1138</v>
+      </c>
+      <c r="C554" s="9" t="s">
+        <v>1138</v>
+      </c>
+      <c r="F554" s="10" t="s">
+        <v>828</v>
+      </c>
+      <c r="J554" s="10" t="s">
+        <v>161</v>
+      </c>
+    </row>
+    <row r="555" spans="2:10" x14ac:dyDescent="0.15">
+      <c r="B555" s="9" t="s">
+        <v>1139</v>
+      </c>
+      <c r="C555" s="9" t="s">
+        <v>1139</v>
+      </c>
+      <c r="F555" s="10" t="s">
+        <v>828</v>
+      </c>
+      <c r="J555" s="10" t="s">
+        <v>161</v>
+      </c>
+    </row>
+    <row r="556" spans="2:10" x14ac:dyDescent="0.15">
+      <c r="B556" s="9" t="s">
+        <v>1140</v>
+      </c>
+      <c r="C556" s="9" t="s">
+        <v>1140</v>
+      </c>
+      <c r="F556" s="10" t="s">
+        <v>828</v>
+      </c>
+      <c r="J556" s="10" t="s">
+        <v>161</v>
+      </c>
+    </row>
+    <row r="557" spans="2:10" x14ac:dyDescent="0.15">
+      <c r="B557" s="9" t="s">
+        <v>1141</v>
+      </c>
+      <c r="C557" s="9" t="s">
+        <v>1141</v>
+      </c>
+      <c r="F557" s="10" t="s">
+        <v>828</v>
+      </c>
+      <c r="J557" s="10" t="s">
+        <v>161</v>
+      </c>
+    </row>
+    <row r="558" spans="2:10" x14ac:dyDescent="0.15">
+      <c r="B558" s="9" t="s">
+        <v>1142</v>
+      </c>
+      <c r="C558" s="9" t="s">
+        <v>1142</v>
+      </c>
+      <c r="F558" s="10" t="s">
+        <v>828</v>
+      </c>
+      <c r="J558" s="10" t="s">
+        <v>161</v>
+      </c>
+    </row>
+    <row r="559" spans="2:10" x14ac:dyDescent="0.15">
+      <c r="B559" s="9" t="s">
+        <v>1143</v>
+      </c>
+      <c r="C559" s="9" t="s">
+        <v>1143</v>
+      </c>
+      <c r="F559" s="10" t="s">
+        <v>828</v>
+      </c>
+      <c r="J559" s="10" t="s">
+        <v>161</v>
+      </c>
+    </row>
+    <row r="560" spans="2:10" x14ac:dyDescent="0.15">
+      <c r="B560" s="9" t="s">
+        <v>1144</v>
+      </c>
+      <c r="C560" s="9" t="s">
+        <v>1144</v>
+      </c>
+      <c r="F560" s="10" t="s">
+        <v>828</v>
+      </c>
+      <c r="J560" s="10" t="s">
+        <v>161</v>
+      </c>
+    </row>
+    <row r="561" spans="2:10" x14ac:dyDescent="0.15">
+      <c r="B561" s="9" t="s">
+        <v>1145</v>
+      </c>
+      <c r="C561" s="9" t="s">
+        <v>1145</v>
+      </c>
+      <c r="F561" s="10" t="s">
+        <v>828</v>
+      </c>
+      <c r="J561" s="10" t="s">
+        <v>161</v>
+      </c>
+    </row>
+    <row r="562" spans="2:10" x14ac:dyDescent="0.15">
+      <c r="B562" s="9" t="s">
+        <v>1146</v>
+      </c>
+      <c r="C562" s="9" t="s">
+        <v>1146</v>
+      </c>
+      <c r="F562" s="10" t="s">
+        <v>828</v>
+      </c>
+      <c r="J562" s="10" t="s">
+        <v>161</v>
+      </c>
+    </row>
+    <row r="563" spans="2:10" x14ac:dyDescent="0.15">
+      <c r="B563" s="9" t="s">
+        <v>1147</v>
+      </c>
+      <c r="C563" s="9" t="s">
+        <v>1147</v>
+      </c>
+      <c r="F563" s="10" t="s">
+        <v>828</v>
+      </c>
+      <c r="J563" s="10" t="s">
+        <v>161</v>
+      </c>
+    </row>
+    <row r="564" spans="2:10" x14ac:dyDescent="0.15">
+      <c r="B564" s="9" t="s">
+        <v>1148</v>
+      </c>
+      <c r="C564" s="9" t="s">
+        <v>1148</v>
+      </c>
+      <c r="F564" s="10" t="s">
+        <v>828</v>
+      </c>
+      <c r="J564" s="10" t="s">
+        <v>161</v>
+      </c>
+    </row>
+    <row r="565" spans="2:10" x14ac:dyDescent="0.15">
+      <c r="B565" s="9" t="s">
+        <v>1149</v>
+      </c>
+      <c r="C565" s="9" t="s">
+        <v>1149</v>
+      </c>
+      <c r="F565" s="10" t="s">
+        <v>828</v>
+      </c>
+      <c r="J565" s="10" t="s">
+        <v>161</v>
+      </c>
+    </row>
+    <row r="566" spans="2:10" x14ac:dyDescent="0.15">
+      <c r="B566" s="9" t="s">
+        <v>1150</v>
+      </c>
+      <c r="C566" s="9" t="s">
+        <v>1150</v>
+      </c>
+      <c r="F566" s="10" t="s">
+        <v>828</v>
+      </c>
+      <c r="J566" s="10" t="s">
+        <v>161</v>
+      </c>
+    </row>
+    <row r="567" spans="2:10" x14ac:dyDescent="0.15">
+      <c r="B567" s="9" t="s">
+        <v>1151</v>
+      </c>
+      <c r="C567" s="9" t="s">
+        <v>1151</v>
+      </c>
+      <c r="F567" s="10" t="s">
+        <v>828</v>
+      </c>
+      <c r="J567" s="10" t="s">
+        <v>161</v>
+      </c>
+    </row>
+    <row r="568" spans="2:10" x14ac:dyDescent="0.15">
+      <c r="B568" s="9" t="s">
+        <v>1152</v>
+      </c>
+      <c r="C568" s="9" t="s">
+        <v>1152</v>
+      </c>
+      <c r="F568" s="10" t="s">
+        <v>828</v>
+      </c>
+      <c r="J568" s="10" t="s">
+        <v>161</v>
+      </c>
+    </row>
+    <row r="569" spans="2:10" x14ac:dyDescent="0.15">
+      <c r="B569" s="9" t="s">
+        <v>1153</v>
+      </c>
+      <c r="C569" s="9" t="s">
+        <v>1153</v>
+      </c>
+      <c r="F569" s="10" t="s">
+        <v>828</v>
+      </c>
+      <c r="J569" s="10" t="s">
+        <v>161</v>
+      </c>
+    </row>
+    <row r="570" spans="2:10" x14ac:dyDescent="0.15">
+      <c r="B570" s="9" t="s">
+        <v>1154</v>
+      </c>
+      <c r="C570" s="9" t="s">
+        <v>1154</v>
+      </c>
+      <c r="F570" s="10" t="s">
+        <v>828</v>
+      </c>
+      <c r="J570" s="10" t="s">
+        <v>161</v>
+      </c>
+    </row>
+    <row r="571" spans="2:10" x14ac:dyDescent="0.15">
+      <c r="B571" s="9" t="s">
+        <v>1155</v>
+      </c>
+      <c r="C571" s="9" t="s">
+        <v>1155</v>
+      </c>
+      <c r="F571" s="10" t="s">
+        <v>828</v>
+      </c>
+      <c r="J571" s="10" t="s">
+        <v>161</v>
+      </c>
+    </row>
+    <row r="572" spans="2:10" x14ac:dyDescent="0.15">
+      <c r="B572" s="9" t="s">
+        <v>1156</v>
+      </c>
+      <c r="C572" s="9" t="s">
+        <v>1156</v>
+      </c>
+      <c r="F572" s="10" t="s">
+        <v>828</v>
+      </c>
+      <c r="J572" s="10" t="s">
+        <v>161</v>
+      </c>
+    </row>
+    <row r="573" spans="2:10" x14ac:dyDescent="0.15">
+      <c r="B573" s="9" t="s">
+        <v>1157</v>
+      </c>
+      <c r="C573" s="9" t="s">
+        <v>1157</v>
+      </c>
+      <c r="F573" s="10" t="s">
+        <v>828</v>
+      </c>
+      <c r="J573" s="10" t="s">
+        <v>161</v>
+      </c>
+    </row>
+    <row r="574" spans="2:10" x14ac:dyDescent="0.15">
+      <c r="B574" s="9" t="s">
+        <v>1158</v>
+      </c>
+      <c r="C574" s="9" t="s">
+        <v>1158</v>
+      </c>
+      <c r="F574" s="10" t="s">
+        <v>828</v>
+      </c>
+      <c r="J574" s="10" t="s">
+        <v>161</v>
+      </c>
+    </row>
+    <row r="575" spans="2:10" x14ac:dyDescent="0.15">
+      <c r="B575" s="9" t="s">
+        <v>1159</v>
+      </c>
+      <c r="C575" s="9" t="s">
+        <v>1159</v>
+      </c>
+      <c r="F575" s="10" t="s">
+        <v>828</v>
+      </c>
+      <c r="J575" s="10" t="s">
+        <v>161</v>
+      </c>
+    </row>
+    <row r="576" spans="2:10" x14ac:dyDescent="0.15">
+      <c r="B576" s="9" t="s">
+        <v>1160</v>
+      </c>
+      <c r="C576" s="9" t="s">
+        <v>1160</v>
+      </c>
+      <c r="F576" s="10" t="s">
+        <v>828</v>
+      </c>
+      <c r="J576" s="10" t="s">
+        <v>161</v>
+      </c>
+    </row>
+    <row r="577" spans="2:10" x14ac:dyDescent="0.15">
+      <c r="B577" s="9" t="s">
+        <v>1161</v>
+      </c>
+      <c r="C577" s="9" t="s">
+        <v>1161</v>
+      </c>
+      <c r="F577" s="10" t="s">
+        <v>828</v>
+      </c>
+      <c r="J577" s="10" t="s">
+        <v>161</v>
+      </c>
+    </row>
+    <row r="578" spans="2:10" x14ac:dyDescent="0.15">
+      <c r="B578" s="9" t="s">
+        <v>1162</v>
+      </c>
+      <c r="C578" s="9" t="s">
+        <v>1162</v>
+      </c>
+      <c r="F578" s="10" t="s">
+        <v>828</v>
+      </c>
+      <c r="J578" s="10" t="s">
+        <v>161</v>
+      </c>
+    </row>
+    <row r="579" spans="2:10" x14ac:dyDescent="0.15">
+      <c r="B579" s="9" t="s">
+        <v>1163</v>
+      </c>
+      <c r="C579" s="9" t="s">
+        <v>1163</v>
+      </c>
+      <c r="F579" s="10" t="s">
+        <v>828</v>
+      </c>
+      <c r="J579" s="10" t="s">
+        <v>161</v>
+      </c>
+    </row>
+    <row r="580" spans="2:10" x14ac:dyDescent="0.15">
+      <c r="B580" s="9" t="s">
+        <v>1164</v>
+      </c>
+      <c r="C580" s="9" t="s">
+        <v>1164</v>
+      </c>
+      <c r="F580" s="10" t="s">
+        <v>828</v>
+      </c>
+      <c r="J580" s="10" t="s">
+        <v>161</v>
+      </c>
+    </row>
+    <row r="581" spans="2:10" x14ac:dyDescent="0.15">
+      <c r="B581" s="9" t="s">
+        <v>1165</v>
+      </c>
+      <c r="C581" s="9" t="s">
+        <v>1165</v>
+      </c>
+      <c r="F581" s="10" t="s">
+        <v>828</v>
+      </c>
+      <c r="J581" s="10" t="s">
+        <v>161</v>
+      </c>
+    </row>
+    <row r="582" spans="2:10" x14ac:dyDescent="0.15">
+      <c r="B582" s="9" t="s">
+        <v>1166</v>
+      </c>
+      <c r="C582" s="9" t="s">
+        <v>1166</v>
+      </c>
+      <c r="F582" s="10" t="s">
+        <v>828</v>
+      </c>
+      <c r="J582" s="10" t="s">
+        <v>161</v>
+      </c>
+    </row>
+    <row r="583" spans="2:10" x14ac:dyDescent="0.15">
+      <c r="B583" s="9" t="s">
+        <v>1167</v>
+      </c>
+      <c r="C583" s="9" t="s">
+        <v>1167</v>
+      </c>
+      <c r="F583" s="10" t="s">
+        <v>828</v>
+      </c>
+      <c r="J583" s="10" t="s">
+        <v>161</v>
+      </c>
+    </row>
+    <row r="584" spans="2:10" x14ac:dyDescent="0.15">
+      <c r="B584" s="9" t="s">
+        <v>1168</v>
+      </c>
+      <c r="C584" s="9" t="s">
+        <v>1168</v>
+      </c>
+      <c r="F584" s="10" t="s">
+        <v>828</v>
+      </c>
+      <c r="J584" s="10" t="s">
+        <v>161</v>
+      </c>
+    </row>
+    <row r="585" spans="2:10" x14ac:dyDescent="0.15">
+      <c r="B585" s="9" t="s">
+        <v>1169</v>
+      </c>
+      <c r="C585" s="9" t="s">
+        <v>1169</v>
+      </c>
+      <c r="F585" s="10" t="s">
+        <v>828</v>
+      </c>
+      <c r="J585" s="10" t="s">
+        <v>161</v>
+      </c>
+    </row>
+    <row r="586" spans="2:10" x14ac:dyDescent="0.15">
+      <c r="B586" s="9" t="s">
+        <v>1170</v>
+      </c>
+      <c r="C586" s="9" t="s">
+        <v>1170</v>
+      </c>
+      <c r="F586" s="10" t="s">
+        <v>828</v>
+      </c>
+      <c r="J586" s="10" t="s">
+        <v>161</v>
+      </c>
+    </row>
+    <row r="587" spans="2:10" x14ac:dyDescent="0.15">
+      <c r="B587" s="9" t="s">
+        <v>1171</v>
+      </c>
+      <c r="C587" s="9" t="s">
+        <v>1171</v>
+      </c>
+      <c r="F587" s="10" t="s">
+        <v>828</v>
+      </c>
+      <c r="J587" s="10" t="s">
+        <v>161</v>
+      </c>
+    </row>
+    <row r="588" spans="2:10" x14ac:dyDescent="0.15">
+      <c r="B588" s="9" t="s">
+        <v>1172</v>
+      </c>
+      <c r="C588" s="9" t="s">
+        <v>1172</v>
+      </c>
+      <c r="F588" s="10" t="s">
+        <v>828</v>
+      </c>
+      <c r="J588" s="10" t="s">
+        <v>161</v>
+      </c>
+    </row>
+    <row r="589" spans="2:10" x14ac:dyDescent="0.15">
+      <c r="B589" s="9" t="s">
+        <v>1173</v>
+      </c>
+      <c r="C589" s="9" t="s">
+        <v>1173</v>
+      </c>
+      <c r="F589" s="10" t="s">
+        <v>828</v>
+      </c>
+      <c r="J589" s="10" t="s">
+        <v>161</v>
+      </c>
+    </row>
+    <row r="590" spans="2:10" x14ac:dyDescent="0.15">
+      <c r="B590" s="9" t="s">
+        <v>1174</v>
+      </c>
+      <c r="C590" s="9" t="s">
+        <v>1174</v>
+      </c>
+      <c r="F590" s="10" t="s">
+        <v>828</v>
+      </c>
+      <c r="J590" s="10" t="s">
+        <v>161</v>
+      </c>
+    </row>
+    <row r="591" spans="2:10" x14ac:dyDescent="0.15">
+      <c r="B591" s="9" t="s">
+        <v>1175</v>
+      </c>
+      <c r="C591" s="9" t="s">
+        <v>1175</v>
+      </c>
+      <c r="F591" s="10" t="s">
+        <v>828</v>
+      </c>
+      <c r="J591" s="10" t="s">
+        <v>161</v>
+      </c>
+    </row>
+    <row r="592" spans="2:10" x14ac:dyDescent="0.15">
+      <c r="B592" s="9" t="s">
+        <v>1176</v>
+      </c>
+      <c r="C592" s="9" t="s">
+        <v>1176</v>
+      </c>
+      <c r="F592" s="10" t="s">
+        <v>828</v>
+      </c>
+      <c r="J592" s="10" t="s">
         <v>161</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Removed MOE SVI data and state fips - double checking the herbicide finding on the server as it's unexpected for total cases.
</commit_message>
<xml_diff>
--- a/data/processed/Data_Dictionary.xlsx
+++ b/data/processed/Data_Dictionary.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/davidmccoy/COVIDxrisk/data/processed/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A5494CF2-1F3C-5F49-AC43-F2E6083A95A3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E54756B2-2C15-E041-A06E-EFC9F2C945E5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-51200" yWindow="0" windowWidth="51200" windowHeight="28800" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="16440" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Table 1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3864" uniqueCount="1305">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3880" uniqueCount="1310">
   <si>
     <t>Col Num</t>
   </si>
@@ -4074,12 +4074,27 @@
   <si>
     <t>Average Arsenic Values</t>
   </si>
+  <si>
+    <t>CYMOXANIL</t>
+  </si>
+  <si>
+    <t>Social.associations.raw.value</t>
+  </si>
+  <si>
+    <t>Residential.segregation...Black.White.raw.value</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Black White Racial Segregation </t>
+  </si>
+  <si>
+    <t>M_UNINSUR</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="6" x14ac:knownFonts="1">
+  <fonts count="8" x14ac:knownFonts="1">
     <font>
       <sz val="10"/>
       <color rgb="FF000000"/>
@@ -4114,6 +4129,18 @@
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Lucida Grande"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color theme="1"/>
+      <name val="Times New Roman"/>
+      <family val="1"/>
     </font>
   </fonts>
   <fills count="2">
@@ -4151,7 +4178,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="14">
+  <cellXfs count="16">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
@@ -4186,6 +4213,10 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -4525,10 +4556,10 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <sheetPr filterMode="1"/>
-  <dimension ref="A1:K592"/>
+  <dimension ref="A1:K601"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A389" zoomScale="87" workbookViewId="0">
-      <selection activeCell="H446" sqref="H446"/>
+    <sheetView tabSelected="1" topLeftCell="A473" zoomScale="87" workbookViewId="0">
+      <selection activeCell="C510" sqref="C510"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="20.19921875" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
@@ -16890,6 +16921,137 @@
       <c r="J592" s="10" t="s">
         <v>161</v>
       </c>
+    </row>
+    <row r="593" spans="2:10" ht="14" x14ac:dyDescent="0.15">
+      <c r="B593" s="14" t="s">
+        <v>1305</v>
+      </c>
+      <c r="C593" s="14" t="s">
+        <v>1305</v>
+      </c>
+      <c r="D593" s="15"/>
+      <c r="E593" s="15"/>
+      <c r="F593" s="15" t="s">
+        <v>828</v>
+      </c>
+      <c r="G593" s="15"/>
+      <c r="H593" s="15"/>
+      <c r="I593" s="15"/>
+      <c r="J593" s="15" t="s">
+        <v>161</v>
+      </c>
+    </row>
+    <row r="594" spans="2:10" ht="14" x14ac:dyDescent="0.15">
+      <c r="B594" s="14" t="s">
+        <v>1306</v>
+      </c>
+      <c r="C594" s="10" t="s">
+        <v>682</v>
+      </c>
+      <c r="D594" s="15"/>
+      <c r="E594" s="15"/>
+      <c r="F594" s="9" t="s">
+        <v>812</v>
+      </c>
+      <c r="G594" s="15"/>
+      <c r="H594" s="15"/>
+      <c r="I594" s="15"/>
+      <c r="J594" s="15" t="s">
+        <v>161</v>
+      </c>
+    </row>
+    <row r="595" spans="2:10" ht="14" x14ac:dyDescent="0.15">
+      <c r="B595" s="14" t="s">
+        <v>1307</v>
+      </c>
+      <c r="C595" s="15" t="s">
+        <v>1308</v>
+      </c>
+      <c r="D595" s="15"/>
+      <c r="E595" s="15"/>
+      <c r="F595" s="15" t="s">
+        <v>856</v>
+      </c>
+      <c r="G595" s="15"/>
+      <c r="H595" s="15"/>
+      <c r="I595" s="15"/>
+      <c r="J595" s="15" t="s">
+        <v>161</v>
+      </c>
+    </row>
+    <row r="596" spans="2:10" ht="14" x14ac:dyDescent="0.15">
+      <c r="B596" s="14" t="s">
+        <v>1309</v>
+      </c>
+      <c r="C596" s="13" t="s">
+        <v>1297</v>
+      </c>
+      <c r="D596" s="15"/>
+      <c r="E596" s="15"/>
+      <c r="F596" s="15" t="s">
+        <v>811</v>
+      </c>
+      <c r="G596" s="15"/>
+      <c r="H596" s="15"/>
+      <c r="I596" s="15"/>
+      <c r="J596" s="15" t="s">
+        <v>162</v>
+      </c>
+    </row>
+    <row r="597" spans="2:10" x14ac:dyDescent="0.15">
+      <c r="B597" s="15"/>
+      <c r="C597" s="15"/>
+      <c r="D597" s="15"/>
+      <c r="E597" s="15"/>
+      <c r="F597" s="15"/>
+      <c r="G597" s="15"/>
+      <c r="H597" s="15"/>
+      <c r="I597" s="15"/>
+      <c r="J597" s="15"/>
+    </row>
+    <row r="598" spans="2:10" x14ac:dyDescent="0.15">
+      <c r="B598" s="15"/>
+      <c r="C598" s="15"/>
+      <c r="D598" s="15"/>
+      <c r="E598" s="15"/>
+      <c r="F598" s="15"/>
+      <c r="G598" s="15"/>
+      <c r="H598" s="15"/>
+      <c r="I598" s="15"/>
+      <c r="J598" s="15"/>
+    </row>
+    <row r="599" spans="2:10" x14ac:dyDescent="0.15">
+      <c r="B599" s="15"/>
+      <c r="C599" s="15"/>
+      <c r="D599" s="15"/>
+      <c r="E599" s="15"/>
+      <c r="F599" s="15"/>
+      <c r="G599" s="15"/>
+      <c r="H599" s="15"/>
+      <c r="I599" s="15"/>
+      <c r="J599" s="15"/>
+    </row>
+    <row r="600" spans="2:10" x14ac:dyDescent="0.15">
+      <c r="B600" s="15"/>
+      <c r="C600" s="15"/>
+      <c r="D600" s="15"/>
+      <c r="E600" s="15"/>
+      <c r="F600" s="15"/>
+      <c r="G600" s="15"/>
+      <c r="H600" s="15"/>
+      <c r="I600" s="15"/>
+      <c r="J600" s="15"/>
+    </row>
+    <row r="601" spans="2:10" x14ac:dyDescent="0.15">
+      <c r="B601" s="15"/>
+      <c r="C601" s="15"/>
+      <c r="D601" s="15"/>
+      <c r="E601" s="15"/>
+      <c r="F601" s="15"/>
+      <c r="G601" s="15"/>
+      <c r="H601" s="15"/>
+      <c r="I601" s="15"/>
+      <c r="J601" s="15"/>
     </row>
   </sheetData>
   <autoFilter ref="A1:K180" xr:uid="{6F8EE88F-6A1E-0944-B4CE-15CC78279902}">

</xml_diff>